<commit_message>
Commented out confusion matrix plot
</commit_message>
<xml_diff>
--- a/data_dump.xlsx
+++ b/data_dump.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\King\cs9414-opinion-mining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271F05A5-8975-47AC-AAA9-230BCEAD42C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69F14BC-F58E-4073-9A4F-29217C5DCE6A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6330" yWindow="2925" windowWidth="20310" windowHeight="11505" activeTab="1" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
+    <workbookView xWindow="32655" yWindow="2505" windowWidth="20310" windowHeight="11505" activeTab="1" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$M$39</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="32">
   <si>
     <t>Classifier</t>
   </si>
@@ -125,6 +128,9 @@
   </si>
   <si>
     <t>further testing shows that it starts to level off at 1000</t>
+  </si>
+  <si>
+    <t>at 1500 MNB_topics test dec train inc</t>
   </si>
 </sst>
 </file>
@@ -782,7 +788,7 @@
   <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,40 +842,40 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2">
-        <v>0.3</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="E2">
-        <v>0.187</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="F2">
-        <v>0.27900000000000003</v>
+        <v>0.26</v>
       </c>
       <c r="G2">
-        <v>0.3</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="H2">
-        <v>0.16300000000000001</v>
+        <v>0.161</v>
       </c>
       <c r="I2">
-        <v>0.3</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="J2">
-        <v>0.3</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="K2">
-        <v>0.16400000000000001</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="L2">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="M2">
-        <v>2.1000000000000001E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -877,40 +883,40 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
       <c r="D3">
-        <v>0.38500000000000001</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="E3">
-        <v>0.24199999999999999</v>
+        <v>0.189</v>
       </c>
       <c r="F3">
-        <v>0.36699999999999999</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="G3">
-        <v>0.38500000000000001</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="H3">
-        <v>0.219</v>
+        <v>0.193</v>
       </c>
       <c r="I3">
-        <v>0.38500000000000001</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="J3">
-        <v>0.38500000000000001</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="K3">
-        <v>0.221</v>
+        <v>0.186</v>
       </c>
       <c r="L3">
-        <v>0.35699999999999998</v>
+        <v>0.318</v>
       </c>
       <c r="M3">
-        <v>2.1999999999999999E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -918,40 +924,40 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="D4">
-        <v>0.28199999999999997</v>
+        <v>0.3</v>
       </c>
       <c r="E4">
-        <v>0.17799999999999999</v>
+        <v>0.187</v>
       </c>
       <c r="F4">
-        <v>0.26</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="G4">
-        <v>0.28199999999999997</v>
+        <v>0.3</v>
       </c>
       <c r="H4">
-        <v>0.161</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="I4">
-        <v>0.28199999999999997</v>
+        <v>0.3</v>
       </c>
       <c r="J4">
-        <v>0.28199999999999997</v>
+        <v>0.3</v>
       </c>
       <c r="K4">
-        <v>0.16200000000000001</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="L4">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="M4">
-        <v>8.9999999999999993E-3</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="O4" t="s">
         <v>28</v>
@@ -962,40 +968,40 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5">
-        <v>0.35099999999999998</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="E5">
-        <v>0.189</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="F5">
-        <v>0.30599999999999999</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="G5">
-        <v>0.35099999999999998</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="H5">
-        <v>0.193</v>
+        <v>0.219</v>
       </c>
       <c r="I5">
-        <v>0.35099999999999998</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="J5">
-        <v>0.35099999999999998</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="K5">
-        <v>0.186</v>
+        <v>0.221</v>
       </c>
       <c r="L5">
-        <v>0.318</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="M5">
-        <v>8.9999999999999993E-3</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1085,40 +1091,40 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
       <c r="D8">
-        <v>0.67200000000000004</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="E8">
-        <v>0.39600000000000002</v>
+        <v>0.433</v>
       </c>
       <c r="F8">
-        <v>0.59</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="G8">
-        <v>0.67200000000000004</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="H8">
-        <v>0.40600000000000003</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="I8">
-        <v>0.67200000000000004</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="J8">
-        <v>0.67200000000000004</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="K8">
-        <v>0.39100000000000001</v>
+        <v>0.41199999999999998</v>
       </c>
       <c r="L8">
-        <v>0.61899999999999999</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="M8">
-        <v>1.4E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -1126,40 +1132,40 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="D9">
-        <v>0.70499999999999996</v>
+        <v>0.69</v>
       </c>
       <c r="E9">
-        <v>0.44</v>
+        <v>0.42299999999999999</v>
       </c>
       <c r="F9">
-        <v>0.63800000000000001</v>
+        <v>0.61199999999999999</v>
       </c>
       <c r="G9">
-        <v>0.70499999999999996</v>
+        <v>0.69</v>
       </c>
       <c r="H9">
-        <v>0.44</v>
+        <v>0.42299999999999999</v>
       </c>
       <c r="I9">
-        <v>0.70499999999999996</v>
+        <v>0.69</v>
       </c>
       <c r="J9">
-        <v>0.70499999999999996</v>
+        <v>0.69</v>
       </c>
       <c r="K9">
-        <v>0.43099999999999999</v>
+        <v>0.41</v>
       </c>
       <c r="L9">
-        <v>0.66</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="M9">
-        <v>1.4E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1167,40 +1173,40 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10">
-        <v>0.70799999999999996</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="E10">
-        <v>0.433</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="F10">
-        <v>0.64600000000000002</v>
+        <v>0.59</v>
       </c>
       <c r="G10">
-        <v>0.70799999999999996</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="H10">
-        <v>0.41899999999999998</v>
+        <v>0.40600000000000003</v>
       </c>
       <c r="I10">
-        <v>0.70799999999999996</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="J10">
-        <v>0.70799999999999996</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="K10">
-        <v>0.41199999999999998</v>
+        <v>0.39100000000000001</v>
       </c>
       <c r="L10">
-        <v>0.66100000000000003</v>
+        <v>0.61899999999999999</v>
       </c>
       <c r="M10">
-        <v>8.0000000000000002E-3</v>
+        <v>1.4E-2</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -1208,40 +1214,40 @@
         <v>8</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11">
-        <v>0.69</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="E11">
-        <v>0.42299999999999999</v>
+        <v>0.44</v>
       </c>
       <c r="F11">
-        <v>0.61199999999999999</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="G11">
-        <v>0.69</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="H11">
-        <v>0.42299999999999999</v>
+        <v>0.44</v>
       </c>
       <c r="I11">
-        <v>0.69</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="J11">
-        <v>0.69</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="K11">
-        <v>0.41</v>
+        <v>0.43099999999999999</v>
       </c>
       <c r="L11">
-        <v>0.63600000000000001</v>
+        <v>0.66</v>
       </c>
       <c r="M11">
-        <v>8.9999999999999993E-3</v>
+        <v>1.4E-2</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -1331,40 +1337,40 @@
         <v>9</v>
       </c>
       <c r="B14">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
       </c>
       <c r="D14">
-        <v>0.32800000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="E14">
-        <v>0.21099999999999999</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="F14">
-        <v>0.312</v>
+        <v>0.27</v>
       </c>
       <c r="G14">
-        <v>0.32800000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="H14">
-        <v>0.18099999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="I14">
-        <v>0.32800000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="J14">
-        <v>0.32800000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="K14">
-        <v>0.184</v>
+        <v>0.155</v>
       </c>
       <c r="L14">
-        <v>0.30499999999999999</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="M14">
-        <v>1.2999999999999999E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -1372,40 +1378,40 @@
         <v>9</v>
       </c>
       <c r="B15">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
       </c>
       <c r="D15">
-        <v>0.50600000000000001</v>
+        <v>0.40699999999999997</v>
       </c>
       <c r="E15">
-        <v>0.47299999999999998</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="F15">
-        <v>0.52100000000000002</v>
+        <v>0.42099999999999999</v>
       </c>
       <c r="G15">
-        <v>0.50600000000000001</v>
+        <v>0.40699999999999997</v>
       </c>
       <c r="H15">
-        <v>0.32600000000000001</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="I15">
-        <v>0.50600000000000001</v>
+        <v>0.40699999999999997</v>
       </c>
       <c r="J15">
-        <v>0.50600000000000001</v>
+        <v>0.40699999999999997</v>
       </c>
       <c r="K15">
-        <v>0.35299999999999998</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="L15">
-        <v>0.48899999999999999</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="M15">
-        <v>1.4E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -1413,40 +1419,40 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
       </c>
       <c r="D16">
-        <v>0.27</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="E16">
-        <v>0.17499999999999999</v>
+        <v>0.21099999999999999</v>
       </c>
       <c r="F16">
-        <v>0.27</v>
+        <v>0.312</v>
       </c>
       <c r="G16">
-        <v>0.27</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="H16">
-        <v>0.15</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="I16">
-        <v>0.27</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="J16">
-        <v>0.27</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="K16">
-        <v>0.155</v>
+        <v>0.184</v>
       </c>
       <c r="L16">
-        <v>0.25700000000000001</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="M16">
-        <v>1.2E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1454,40 +1460,40 @@
         <v>9</v>
       </c>
       <c r="B17">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
       </c>
       <c r="D17">
-        <v>0.40699999999999997</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="E17">
-        <v>0.36699999999999999</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="F17">
-        <v>0.42099999999999999</v>
+        <v>0.52100000000000002</v>
       </c>
       <c r="G17">
-        <v>0.40699999999999997</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="H17">
-        <v>0.26300000000000001</v>
+        <v>0.32600000000000001</v>
       </c>
       <c r="I17">
-        <v>0.40699999999999997</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="J17">
-        <v>0.40699999999999997</v>
+        <v>0.50600000000000001</v>
       </c>
       <c r="K17">
-        <v>0.28599999999999998</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="L17">
-        <v>0.39600000000000002</v>
+        <v>0.48899999999999999</v>
       </c>
       <c r="M17">
-        <v>1.2999999999999999E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="O17" t="s">
         <v>29</v>
@@ -1498,40 +1504,40 @@
         <v>9</v>
       </c>
       <c r="B18">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
       </c>
       <c r="D18">
-        <v>0.33600000000000002</v>
+        <v>0.35</v>
       </c>
       <c r="E18">
-        <v>0.20399999999999999</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="F18">
-        <v>0.34499999999999997</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="G18">
-        <v>0.33600000000000002</v>
+        <v>0.35</v>
       </c>
       <c r="H18">
-        <v>0.159</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="I18">
-        <v>0.33600000000000002</v>
+        <v>0.35</v>
       </c>
       <c r="J18">
-        <v>0.33600000000000002</v>
+        <v>0.35</v>
       </c>
       <c r="K18">
-        <v>0.156</v>
+        <v>0.17</v>
       </c>
       <c r="L18">
-        <v>0.29199999999999998</v>
+        <v>0.313</v>
       </c>
       <c r="M18">
-        <v>2.7E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1539,40 +1545,40 @@
         <v>9</v>
       </c>
       <c r="B19">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
       </c>
       <c r="D19">
-        <v>0.56899999999999995</v>
+        <v>0.58099999999999996</v>
       </c>
       <c r="E19">
-        <v>0.38300000000000001</v>
+        <v>0.48699999999999999</v>
       </c>
       <c r="F19">
-        <v>0.55300000000000005</v>
+        <v>0.59599999999999997</v>
       </c>
       <c r="G19">
-        <v>0.56899999999999995</v>
+        <v>0.58099999999999996</v>
       </c>
       <c r="H19">
-        <v>0.28999999999999998</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="I19">
-        <v>0.56899999999999995</v>
+        <v>0.58099999999999996</v>
       </c>
       <c r="J19">
-        <v>0.56899999999999995</v>
+        <v>0.58099999999999996</v>
       </c>
       <c r="K19">
-        <v>0.28699999999999998</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="L19">
-        <v>0.51600000000000001</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="M19">
-        <v>4.0300000000000002E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -1580,40 +1586,40 @@
         <v>9</v>
       </c>
       <c r="B20">
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
       <c r="D20">
-        <v>0.35</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="E20">
-        <v>0.19500000000000001</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="F20">
-        <v>0.33200000000000002</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="G20">
-        <v>0.35</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="H20">
-        <v>0.17599999999999999</v>
+        <v>0.159</v>
       </c>
       <c r="I20">
-        <v>0.35</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="J20">
-        <v>0.35</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="K20">
-        <v>0.17</v>
+        <v>0.156</v>
       </c>
       <c r="L20">
-        <v>0.313</v>
+        <v>0.29199999999999998</v>
       </c>
       <c r="M20">
-        <v>3.2000000000000001E-2</v>
+        <v>2.7E-2</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1621,40 +1627,40 @@
         <v>9</v>
       </c>
       <c r="B21">
-        <v>600</v>
+        <v>900</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
       </c>
       <c r="D21">
-        <v>0.58099999999999996</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="E21">
-        <v>0.48699999999999999</v>
+        <v>0.38300000000000001</v>
       </c>
       <c r="F21">
-        <v>0.59599999999999997</v>
+        <v>0.55300000000000005</v>
       </c>
       <c r="G21">
-        <v>0.58099999999999996</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="H21">
-        <v>0.32400000000000001</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="I21">
-        <v>0.58099999999999996</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="J21">
-        <v>0.58099999999999996</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="K21">
-        <v>0.33200000000000002</v>
+        <v>0.28699999999999998</v>
       </c>
       <c r="L21">
-        <v>0.54200000000000004</v>
+        <v>0.51600000000000001</v>
       </c>
       <c r="M21">
-        <v>3.7999999999999999E-2</v>
+        <v>4.0300000000000002E-2</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1744,40 +1750,40 @@
         <v>10</v>
       </c>
       <c r="B24">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="D24">
-        <v>0.71599999999999997</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="E24">
-        <v>0.65100000000000002</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="F24">
-        <v>0.70899999999999996</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="G24">
-        <v>0.71599999999999997</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="H24">
-        <v>0.54400000000000004</v>
+        <v>0.53700000000000003</v>
       </c>
       <c r="I24">
-        <v>0.71599999999999997</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="J24">
-        <v>0.71599999999999997</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="K24">
-        <v>0.57199999999999995</v>
+        <v>0.55800000000000005</v>
       </c>
       <c r="L24">
-        <v>0.70599999999999996</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="M24">
-        <v>1.7000000000000001E-2</v>
+        <v>9.7999999999999997E-3</v>
       </c>
       <c r="O24" t="s">
         <v>30</v>
@@ -1788,40 +1794,40 @@
         <v>10</v>
       </c>
       <c r="B25">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="C25" t="s">
         <v>15</v>
       </c>
       <c r="D25">
-        <v>0.78500000000000003</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="E25">
-        <v>0.752</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="F25">
-        <v>0.78100000000000003</v>
+        <v>0.75</v>
       </c>
       <c r="G25">
-        <v>0.78500000000000003</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="H25">
-        <v>0.66800000000000004</v>
+        <v>0.64700000000000002</v>
       </c>
       <c r="I25">
-        <v>0.78500000000000003</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="J25">
-        <v>0.78500000000000003</v>
+        <v>0.75700000000000001</v>
       </c>
       <c r="K25">
-        <v>0.69899999999999995</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="L25">
-        <v>0.78</v>
+        <v>0.751</v>
       </c>
       <c r="M25">
-        <v>2.1999999999999999E-2</v>
+        <v>1.18E-2</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -1829,40 +1835,40 @@
         <v>10</v>
       </c>
       <c r="B26">
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
       </c>
       <c r="D26">
-        <v>0.73199999999999998</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="E26">
-        <v>0.73199999999999998</v>
+        <v>0.65100000000000002</v>
       </c>
       <c r="F26">
-        <v>0.73799999999999999</v>
+        <v>0.70899999999999996</v>
       </c>
       <c r="G26">
-        <v>0.73199999999999998</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="H26">
-        <v>0.52500000000000002</v>
+        <v>0.54400000000000004</v>
       </c>
       <c r="I26">
-        <v>0.73199999999999998</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="J26">
-        <v>0.73199999999999998</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="K26">
-        <v>0.54500000000000004</v>
+        <v>0.57199999999999995</v>
       </c>
       <c r="L26">
-        <v>0.71399999999999997</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="M26">
-        <v>0.04</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -1870,87 +1876,992 @@
         <v>10</v>
       </c>
       <c r="B27">
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="C27" t="s">
         <v>15</v>
       </c>
       <c r="D27">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="E27">
+        <v>0.752</v>
+      </c>
+      <c r="F27">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="G27">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="H27">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="I27">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="J27">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="K27">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="L27">
+        <v>0.78</v>
+      </c>
+      <c r="M27">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>1000</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="E28">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="F28">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="G28">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="H28">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="I28">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="J28">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="K28">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="L28">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="M28">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>1000</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29">
         <v>0.84499999999999997</v>
       </c>
-      <c r="E27">
+      <c r="E29">
         <v>0.85399999999999998</v>
       </c>
-      <c r="F27">
+      <c r="F29">
         <v>0.84799999999999998</v>
       </c>
-      <c r="G27">
+      <c r="G29">
         <v>0.84499999999999997</v>
       </c>
-      <c r="H27">
+      <c r="H29">
         <v>0.70699999999999996</v>
       </c>
-      <c r="I27">
+      <c r="I29">
         <v>0.84499999999999997</v>
       </c>
-      <c r="J27">
+      <c r="J29">
         <v>0.84499999999999997</v>
       </c>
-      <c r="K27">
+      <c r="K29">
         <v>0.747</v>
       </c>
-      <c r="L27">
+      <c r="L29">
         <v>0.83899999999999997</v>
       </c>
-      <c r="M27">
+      <c r="M29">
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <v>100</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30">
+        <v>0.254</v>
+      </c>
+      <c r="E30">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="F30">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="G30">
+        <v>0.254</v>
+      </c>
+      <c r="H30">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="I30">
+        <v>0.254</v>
+      </c>
+      <c r="J30">
+        <v>0.254</v>
+      </c>
+      <c r="K30">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="L30">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="M30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31">
+        <v>100</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="E31">
+        <v>0.4</v>
+      </c>
+      <c r="F31">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="G31">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="H31">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="I31">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="J31">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="K31">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="L31">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="M31">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32">
+        <v>200</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="E32">
+        <v>0.219</v>
+      </c>
+      <c r="F32">
+        <v>0.314</v>
+      </c>
+      <c r="G32">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="H32">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="I32">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="J32">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="K32">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="L32">
+        <v>0.31</v>
+      </c>
+      <c r="M32">
+        <v>0.01</v>
+      </c>
+      <c r="O32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33">
+        <v>200</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="E33">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="F33">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="G33">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="H33">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="I33">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="J33">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="K33">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="L33">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="M33">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>400</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="E34">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="F34">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="G34">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="H34">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="I34">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="J34">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="K34">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="L34">
+        <v>0.34</v>
+      </c>
+      <c r="M34">
+        <v>9.5999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>400</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>0.622</v>
+      </c>
+      <c r="E35">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="F35">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="G35">
+        <v>0.622</v>
+      </c>
+      <c r="H35">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="I35">
+        <v>0.622</v>
+      </c>
+      <c r="J35">
+        <v>0.622</v>
+      </c>
+      <c r="K35">
+        <v>0.497</v>
+      </c>
+      <c r="L35">
+        <v>0.61</v>
+      </c>
+      <c r="M35">
+        <v>1.1599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>1000</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="E36">
+        <v>0.216</v>
+      </c>
+      <c r="F36">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="G36">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="H36">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="I36">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="J36">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="K36">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="L36">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="M36">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37">
+        <v>1000</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="E37">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="F37">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="G37">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="H37">
+        <v>0.501</v>
+      </c>
+      <c r="I37">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="J37">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="K37">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="L37">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="M37">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38">
+        <v>1500</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="E38">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="F38">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="G38">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="H38">
+        <v>0.18</v>
+      </c>
+      <c r="I38">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="J38">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="K38">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="L38">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="M38">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39">
+        <v>1500</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="E39">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="F39">
+        <v>0.74</v>
+      </c>
+      <c r="G39">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="H39">
+        <v>0.497</v>
+      </c>
+      <c r="I39">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="J39">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="K39">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="L39">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="M39">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40">
+        <v>100</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="E40">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F40">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="G40">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="H40">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="I40">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="J40">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="K40">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="L40">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="M40">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41">
+        <v>100</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="E41">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="F41">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="G41">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="H41">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="I41">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="J41">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="K41">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="L41">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="M41">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42">
+        <v>200</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="E42">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="F42">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="G42">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="H42">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="I42">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="J42">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="K42">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="L42">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="M42">
+        <v>6.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <v>200</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="E43">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="F43">
+        <v>0.748</v>
+      </c>
+      <c r="G43">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="H43">
+        <v>0.629</v>
+      </c>
+      <c r="I43">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="J43">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="K43">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="L43">
+        <v>0.749</v>
+      </c>
+      <c r="M43">
+        <v>8.5000000000000006E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44">
+        <v>400</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="E44">
+        <v>0.68899999999999995</v>
+      </c>
+      <c r="F44">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="G44">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="H44">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="I44">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="J44">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="K44">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="L44">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="M44">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45">
+        <v>400</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="E45">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="F45">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="G45">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="H45">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="I45">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="J45">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="K45">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="L45">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="M45">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <v>1000</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46">
+        <v>0.746</v>
+      </c>
+      <c r="E46">
+        <v>0.7</v>
+      </c>
+      <c r="F46">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="G46">
+        <v>0.746</v>
+      </c>
+      <c r="H46">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="I46">
+        <v>0.746</v>
+      </c>
+      <c r="J46">
+        <v>0.746</v>
+      </c>
+      <c r="K46">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="L46">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="M46">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47">
+        <v>1000</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="E47">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="F47">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="G47">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="H47">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="I47">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="J47">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="K47">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="L47">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="M47">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48">
+        <v>1500</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="E48">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="F48">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="G48">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="H48">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="I48">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="J48">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="K48">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="L48">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="M48">
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49">
+        <v>1500</v>
+      </c>
+      <c r="C49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="E49">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="F49">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="G49">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="H49">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="I49">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="J49">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="K49">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="L49">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="M49">
+        <v>2.9499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B58" s="3"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B61" s="3"/>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B62" s="3"/>
       <c r="C62" s="2"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B63" s="3"/>
       <c r="C63" s="2"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B64" s="3"/>
       <c r="C64" s="2"/>
     </row>
@@ -1991,6 +2902,7 @@
       <c r="C73" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M37" xr:uid="{3BBEE31F-A494-4277-82AD-63F056B36783}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed q2 table data and q4 graphs
</commit_message>
<xml_diff>
--- a/data_dump.xlsx
+++ b/data_dump.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doodey\cs9414-opinion-mining\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\King\cs9414-opinion-mining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A667858-A846-4516-AC0E-580ED1021B88}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F67372-9FAA-4E93-A281-C99C20380AD1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA61A77C-51F7-4D98-BF60-5DD3CA46162A}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -1026,11 +1026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFAC374A-F1AE-473F-9409-AFFE657A853B}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:L42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,7 +1078,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1120,7 +1119,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1205,7 +1204,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1246,7 +1245,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1287,7 +1286,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1328,7 +1327,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1339,37 +1338,37 @@
         <v>14</v>
       </c>
       <c r="D8">
-        <v>0.70799999999999996</v>
+        <v>0.66</v>
       </c>
       <c r="E8">
-        <v>0.433</v>
+        <v>0.44400000000000001</v>
       </c>
       <c r="F8">
-        <v>0.64600000000000002</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="G8">
-        <v>0.70799999999999996</v>
+        <v>0.66</v>
       </c>
       <c r="H8">
-        <v>0.41899999999999998</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="I8">
-        <v>0.70799999999999996</v>
+        <v>0.66</v>
       </c>
       <c r="J8">
-        <v>0.70799999999999996</v>
+        <v>0.66</v>
       </c>
       <c r="K8">
-        <v>0.41199999999999998</v>
+        <v>0.39900000000000002</v>
       </c>
       <c r="L8">
-        <v>0.66100000000000003</v>
+        <v>0.625</v>
       </c>
       <c r="M8">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1380,34 +1379,34 @@
         <v>15</v>
       </c>
       <c r="D9">
-        <v>0.69</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="E9">
-        <v>0.42299999999999999</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="F9">
-        <v>0.61199999999999999</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="G9">
-        <v>0.69</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="H9">
-        <v>0.42299999999999999</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="I9">
-        <v>0.69</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="J9">
-        <v>0.69</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="K9">
-        <v>0.41</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="L9">
-        <v>0.63600000000000001</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="M9">
-        <v>8.9999999999999993E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -1424,16 +1423,16 @@
         <v>0.67200000000000004</v>
       </c>
       <c r="E10">
-        <v>0.39600000000000002</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="F10">
-        <v>0.59</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="G10">
         <v>0.67200000000000004</v>
       </c>
       <c r="H10">
-        <v>0.40600000000000003</v>
+        <v>0.41</v>
       </c>
       <c r="I10">
         <v>0.67200000000000004</v>
@@ -1442,16 +1441,16 @@
         <v>0.67200000000000004</v>
       </c>
       <c r="K10">
-        <v>0.39100000000000001</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="L10">
-        <v>0.61899999999999999</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="M10">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1462,37 +1461,37 @@
         <v>15</v>
       </c>
       <c r="D11">
-        <v>0.70499999999999996</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="E11">
-        <v>0.44</v>
+        <v>0.57699999999999996</v>
       </c>
       <c r="F11">
-        <v>0.63800000000000001</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="G11">
-        <v>0.70499999999999996</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="H11">
-        <v>0.44</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="I11">
-        <v>0.70499999999999996</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="J11">
-        <v>0.70499999999999996</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="K11">
-        <v>0.43099999999999999</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="L11">
-        <v>0.66</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="M11">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1503,37 +1502,37 @@
         <v>14</v>
       </c>
       <c r="D12">
-        <v>0.65</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="E12">
-        <v>0.39200000000000002</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="F12">
-        <v>0.57299999999999995</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="G12">
-        <v>0.65</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="H12">
-        <v>0.39500000000000002</v>
+        <v>0.41</v>
       </c>
       <c r="I12">
-        <v>0.65</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="J12">
-        <v>0.65</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="K12">
-        <v>0.377</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="L12">
-        <v>0.59099999999999997</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="M12">
-        <v>2.8000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1544,37 +1543,37 @@
         <v>15</v>
       </c>
       <c r="D13">
-        <v>0.70299999999999996</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="E13">
-        <v>0.435</v>
+        <v>0.57699999999999996</v>
       </c>
       <c r="F13">
-        <v>0.63200000000000001</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="G13">
-        <v>0.70299999999999996</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="H13">
-        <v>0.42699999999999999</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="I13">
-        <v>0.70299999999999996</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="J13">
-        <v>0.70299999999999996</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="K13">
-        <v>0.41799999999999998</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="L13">
-        <v>0.65200000000000002</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="M13">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1615,7 +1614,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1697,7 +1696,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1741,7 +1740,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1782,7 +1781,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1823,7 +1822,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1864,7 +1863,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1905,7 +1904,7 @@
         <v>4.0300000000000002E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1946,7 +1945,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2031,7 +2030,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -2072,7 +2071,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2113,7 +2112,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2154,7 +2153,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2195,7 +2194,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2236,7 +2235,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -2277,7 +2276,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -2362,7 +2361,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -2403,7 +2402,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -2444,7 +2443,7 @@
         <v>9.5999999999999992E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2485,7 +2484,7 @@
         <v>1.1599999999999999E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2526,7 +2525,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2567,7 +2566,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2608,7 +2607,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2649,7 +2648,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -2690,7 +2689,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -2772,7 +2771,7 @@
         <v>6.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -2813,7 +2812,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -2854,7 +2853,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -2895,7 +2894,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -2936,7 +2935,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -2977,7 +2976,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -3018,7 +3017,7 @@
         <v>2.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -3144,18 +3143,7 @@
       <c r="C73" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M49" xr:uid="{3BBEE31F-A494-4277-82AD-63F056B36783}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="200"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="test"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M49" xr:uid="{3BBEE31F-A494-4277-82AD-63F056B36783}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
table for part 1 of q5
</commit_message>
<xml_diff>
--- a/data_dump.xlsx
+++ b/data_dump.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\King\cs9414-opinion-mining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F67372-9FAA-4E93-A281-C99C20380AD1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104A731E-6B64-4C12-8710-9301F929BF52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Q5" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$M$49</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="42">
   <si>
     <t>Classifier</t>
   </si>
@@ -131,6 +132,36 @@
   </si>
   <si>
     <t>at 1500 MNB_topics test dec train inc</t>
+  </si>
+  <si>
+    <t>precision</t>
+  </si>
+  <si>
+    <t>recall</t>
+  </si>
+  <si>
+    <t>f1-score</t>
+  </si>
+  <si>
+    <t>support</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>micro</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>macro</t>
+  </si>
+  <si>
+    <t>weighted</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFAC374A-F1AE-473F-9409-AFFE657A853B}">
   <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
@@ -3147,4 +3178,916 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96611E49-C074-44E2-ADBF-AAB639D2C6AE}">
+  <dimension ref="A1:M64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>0.91</v>
+      </c>
+      <c r="E3">
+        <v>0.99</v>
+      </c>
+      <c r="F3">
+        <v>0.95</v>
+      </c>
+      <c r="G3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>0.62</v>
+      </c>
+      <c r="E4">
+        <v>0.2</v>
+      </c>
+      <c r="F4">
+        <v>0.3</v>
+      </c>
+      <c r="G4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6">
+        <v>0.9</v>
+      </c>
+      <c r="E6">
+        <v>0.9</v>
+      </c>
+      <c r="F6">
+        <v>0.9</v>
+      </c>
+      <c r="G6">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>0.76</v>
+      </c>
+      <c r="E7">
+        <v>0.59</v>
+      </c>
+      <c r="F7">
+        <v>0.62</v>
+      </c>
+      <c r="G7">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8">
+        <v>0.88</v>
+      </c>
+      <c r="E8">
+        <v>0.9</v>
+      </c>
+      <c r="F8">
+        <v>0.88</v>
+      </c>
+      <c r="G8">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12">
+        <v>0.92</v>
+      </c>
+      <c r="E12">
+        <v>0.98</v>
+      </c>
+      <c r="F12">
+        <v>0.95</v>
+      </c>
+      <c r="G12">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13">
+        <v>0.65</v>
+      </c>
+      <c r="E13">
+        <v>0.25</v>
+      </c>
+      <c r="F13">
+        <v>0.36</v>
+      </c>
+      <c r="G13">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15">
+        <v>0.91</v>
+      </c>
+      <c r="E15">
+        <v>0.91</v>
+      </c>
+      <c r="F15">
+        <v>0.91</v>
+      </c>
+      <c r="G15">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16">
+        <v>0.78</v>
+      </c>
+      <c r="E16">
+        <v>0.62</v>
+      </c>
+      <c r="F16">
+        <v>0.65</v>
+      </c>
+      <c r="G16">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17">
+        <v>0.89</v>
+      </c>
+      <c r="E17">
+        <v>0.91</v>
+      </c>
+      <c r="F17">
+        <v>0.89</v>
+      </c>
+      <c r="G17">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>200</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="E19">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="F19">
+        <v>0.88</v>
+      </c>
+      <c r="G19">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="H19">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="I19">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="J19">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="K19">
+        <v>0.624</v>
+      </c>
+      <c r="L19">
+        <v>0.878</v>
+      </c>
+      <c r="M19">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>200</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="E20">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="F20">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="G20">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="H20">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="I20">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="J20">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="K20">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="L20">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="M20">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25">
+        <v>0.93</v>
+      </c>
+      <c r="E25">
+        <v>0.97</v>
+      </c>
+      <c r="F25">
+        <v>0.95</v>
+      </c>
+      <c r="G25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E26">
+        <v>0.35</v>
+      </c>
+      <c r="F26">
+        <v>0.43</v>
+      </c>
+      <c r="G26">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28">
+        <v>0.9</v>
+      </c>
+      <c r="E28">
+        <v>0.9</v>
+      </c>
+      <c r="F28">
+        <v>0.9</v>
+      </c>
+      <c r="G28">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29">
+        <v>0.74</v>
+      </c>
+      <c r="E29">
+        <v>0.66</v>
+      </c>
+      <c r="F29">
+        <v>0.69</v>
+      </c>
+      <c r="G29">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30">
+        <v>0.89</v>
+      </c>
+      <c r="E30">
+        <v>0.9</v>
+      </c>
+      <c r="F30">
+        <v>0.89</v>
+      </c>
+      <c r="G30">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34">
+        <v>0.94</v>
+      </c>
+      <c r="E34">
+        <v>0.96</v>
+      </c>
+      <c r="F34">
+        <v>0.95</v>
+      </c>
+      <c r="G34">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35">
+        <v>0.61</v>
+      </c>
+      <c r="E35">
+        <v>0.51</v>
+      </c>
+      <c r="F35">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37">
+        <v>0.91</v>
+      </c>
+      <c r="E37">
+        <v>0.91</v>
+      </c>
+      <c r="F37">
+        <v>0.91</v>
+      </c>
+      <c r="G37">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38">
+        <v>0.78</v>
+      </c>
+      <c r="E38">
+        <v>0.74</v>
+      </c>
+      <c r="F38">
+        <v>0.76</v>
+      </c>
+      <c r="G38">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39">
+        <v>0.91</v>
+      </c>
+      <c r="E39">
+        <v>0.91</v>
+      </c>
+      <c r="F39">
+        <v>0.91</v>
+      </c>
+      <c r="G39">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41">
+        <v>200</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="E41">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="F41">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="G41">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="H41">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="I41">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="J41">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="K41">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="L41">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="M41">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42">
+        <v>200</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="E42">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="F42">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="G42">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="H42">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="I42">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="J42">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="K42">
+        <v>0.755</v>
+      </c>
+      <c r="L42">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="M42">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47">
+        <v>0.92</v>
+      </c>
+      <c r="E47">
+        <v>0.97</v>
+      </c>
+      <c r="F47">
+        <v>0.94</v>
+      </c>
+      <c r="G47">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D48">
+        <v>0.52</v>
+      </c>
+      <c r="E48">
+        <v>0.3</v>
+      </c>
+      <c r="F48">
+        <v>0.38</v>
+      </c>
+      <c r="G48">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50">
+        <v>0.9</v>
+      </c>
+      <c r="E50">
+        <v>0.9</v>
+      </c>
+      <c r="F50">
+        <v>0.9</v>
+      </c>
+      <c r="G50">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51">
+        <v>0.72</v>
+      </c>
+      <c r="E51">
+        <v>0.63</v>
+      </c>
+      <c r="F51">
+        <v>0.66</v>
+      </c>
+      <c r="G51">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52">
+        <v>0.88</v>
+      </c>
+      <c r="E52">
+        <v>0.9</v>
+      </c>
+      <c r="F52">
+        <v>0.88</v>
+      </c>
+      <c r="G52">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56">
+        <v>0.94</v>
+      </c>
+      <c r="E56">
+        <v>0.97</v>
+      </c>
+      <c r="F56">
+        <v>0.95</v>
+      </c>
+      <c r="G56">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>37</v>
+      </c>
+      <c r="D57">
+        <v>0.64</v>
+      </c>
+      <c r="E57">
+        <v>0.5</v>
+      </c>
+      <c r="F57">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G57">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59">
+        <v>0.92</v>
+      </c>
+      <c r="E59">
+        <v>0.92</v>
+      </c>
+      <c r="F59">
+        <v>0.92</v>
+      </c>
+      <c r="G59">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60" t="s">
+        <v>39</v>
+      </c>
+      <c r="D60">
+        <v>0.79</v>
+      </c>
+      <c r="E60">
+        <v>0.74</v>
+      </c>
+      <c r="F60">
+        <v>0.76</v>
+      </c>
+      <c r="G60">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61">
+        <v>0.91</v>
+      </c>
+      <c r="E61">
+        <v>0.92</v>
+      </c>
+      <c r="F61">
+        <v>0.91</v>
+      </c>
+      <c r="G61">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63">
+        <v>200</v>
+      </c>
+      <c r="C63" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="E63">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="F63">
+        <v>0.878</v>
+      </c>
+      <c r="G63">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="H63">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="I63">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="J63">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="K63">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="L63">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="M63">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64">
+        <v>200</v>
+      </c>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="E64">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="F64">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="G64">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="H64">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="I64">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="J64">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="K64">
+        <v>0.76</v>
+      </c>
+      <c r="L64">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="M64">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Data completed to be put in words
</commit_message>
<xml_diff>
--- a/data_dump.xlsx
+++ b/data_dump.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\King\cs9414-opinion-mining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104A731E-6B64-4C12-8710-9301F929BF52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF0CF5E-542B-44A0-8F35-89919D8BF2CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="46">
   <si>
     <t>Classifier</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>weighted</t>
+  </si>
+  <si>
+    <t>neutral</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>seconds</t>
   </si>
 </sst>
 </file>
@@ -3182,10 +3194,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96611E49-C074-44E2-ADBF-AAB639D2C6AE}">
-  <dimension ref="A1:M64"/>
+  <dimension ref="A1:W148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="M135" sqref="M135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4087,6 +4099,1365 @@
         <v>2.7E-2</v>
       </c>
     </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>32</v>
+      </c>
+      <c r="C68" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" t="s">
+        <v>35</v>
+      </c>
+      <c r="J68" t="s">
+        <v>32</v>
+      </c>
+      <c r="K68" t="s">
+        <v>33</v>
+      </c>
+      <c r="L68" t="s">
+        <v>34</v>
+      </c>
+      <c r="M68" t="s">
+        <v>35</v>
+      </c>
+      <c r="R68" t="s">
+        <v>32</v>
+      </c>
+      <c r="S68" t="s">
+        <v>33</v>
+      </c>
+      <c r="T68" t="s">
+        <v>34</v>
+      </c>
+      <c r="U68" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70">
+        <v>0.96</v>
+      </c>
+      <c r="D70">
+        <v>0.47</v>
+      </c>
+      <c r="E70">
+        <v>0.63</v>
+      </c>
+      <c r="F70">
+        <v>1294</v>
+      </c>
+      <c r="J70" t="s">
+        <v>36</v>
+      </c>
+      <c r="K70">
+        <v>0.95</v>
+      </c>
+      <c r="L70">
+        <v>0.46</v>
+      </c>
+      <c r="M70">
+        <v>0.62</v>
+      </c>
+      <c r="N70">
+        <v>335</v>
+      </c>
+      <c r="R70" t="s">
+        <v>36</v>
+      </c>
+      <c r="S70">
+        <v>0.96</v>
+      </c>
+      <c r="T70">
+        <v>0.48</v>
+      </c>
+      <c r="U70">
+        <v>0.64</v>
+      </c>
+      <c r="V70">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>42</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="J71" t="s">
+        <v>42</v>
+      </c>
+      <c r="K71">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="R71" t="s">
+        <v>42</v>
+      </c>
+      <c r="S71">
+        <v>0</v>
+      </c>
+      <c r="T71">
+        <v>0</v>
+      </c>
+      <c r="U71">
+        <v>0</v>
+      </c>
+      <c r="V71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>37</v>
+      </c>
+      <c r="C72">
+        <v>0.18</v>
+      </c>
+      <c r="D72">
+        <v>0.61</v>
+      </c>
+      <c r="E72">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F72">
+        <v>153</v>
+      </c>
+      <c r="J72" t="s">
+        <v>37</v>
+      </c>
+      <c r="K72">
+        <v>0.2</v>
+      </c>
+      <c r="L72">
+        <v>0.62</v>
+      </c>
+      <c r="M72">
+        <v>0.3</v>
+      </c>
+      <c r="N72">
+        <v>40</v>
+      </c>
+      <c r="R72" t="s">
+        <v>37</v>
+      </c>
+      <c r="S72">
+        <v>0.18</v>
+      </c>
+      <c r="T72">
+        <v>0.61</v>
+      </c>
+      <c r="U72">
+        <v>0.27</v>
+      </c>
+      <c r="V72">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>38</v>
+      </c>
+      <c r="C74" t="s">
+        <v>39</v>
+      </c>
+      <c r="D74">
+        <v>0.49</v>
+      </c>
+      <c r="E74">
+        <v>0.49</v>
+      </c>
+      <c r="F74">
+        <v>0.49</v>
+      </c>
+      <c r="G74">
+        <v>1447</v>
+      </c>
+      <c r="J74" t="s">
+        <v>38</v>
+      </c>
+      <c r="K74" t="s">
+        <v>39</v>
+      </c>
+      <c r="L74">
+        <v>0.47</v>
+      </c>
+      <c r="M74">
+        <v>0.47</v>
+      </c>
+      <c r="N74">
+        <v>0.47</v>
+      </c>
+      <c r="O74">
+        <v>375</v>
+      </c>
+      <c r="R74" t="s">
+        <v>38</v>
+      </c>
+      <c r="S74" t="s">
+        <v>39</v>
+      </c>
+      <c r="T74">
+        <v>0.49</v>
+      </c>
+      <c r="U74">
+        <v>0.49</v>
+      </c>
+      <c r="V74">
+        <v>0.49</v>
+      </c>
+      <c r="W74">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>40</v>
+      </c>
+      <c r="C75" t="s">
+        <v>39</v>
+      </c>
+      <c r="D75">
+        <v>0.38</v>
+      </c>
+      <c r="E75">
+        <v>0.36</v>
+      </c>
+      <c r="F75">
+        <v>0.3</v>
+      </c>
+      <c r="G75">
+        <v>1447</v>
+      </c>
+      <c r="J75" t="s">
+        <v>40</v>
+      </c>
+      <c r="K75" t="s">
+        <v>39</v>
+      </c>
+      <c r="L75">
+        <v>0.38</v>
+      </c>
+      <c r="M75">
+        <v>0.36</v>
+      </c>
+      <c r="N75">
+        <v>0.31</v>
+      </c>
+      <c r="O75">
+        <v>375</v>
+      </c>
+      <c r="R75" t="s">
+        <v>40</v>
+      </c>
+      <c r="S75" t="s">
+        <v>39</v>
+      </c>
+      <c r="T75">
+        <v>0.38</v>
+      </c>
+      <c r="U75">
+        <v>0.36</v>
+      </c>
+      <c r="V75">
+        <v>0.3</v>
+      </c>
+      <c r="W75">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>41</v>
+      </c>
+      <c r="B76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C76">
+        <v>0.88</v>
+      </c>
+      <c r="D76">
+        <v>0.49</v>
+      </c>
+      <c r="E76">
+        <v>0.59</v>
+      </c>
+      <c r="F76">
+        <v>1447</v>
+      </c>
+      <c r="I76" t="s">
+        <v>41</v>
+      </c>
+      <c r="J76" t="s">
+        <v>39</v>
+      </c>
+      <c r="K76">
+        <v>0.87</v>
+      </c>
+      <c r="L76">
+        <v>0.47</v>
+      </c>
+      <c r="M76">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="N76">
+        <v>375</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>41</v>
+      </c>
+      <c r="R76" t="s">
+        <v>39</v>
+      </c>
+      <c r="S76">
+        <v>0.88</v>
+      </c>
+      <c r="T76">
+        <v>0.49</v>
+      </c>
+      <c r="U76">
+        <v>0.6</v>
+      </c>
+      <c r="V76">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>0.48652384243261898</v>
+      </c>
+      <c r="I78">
+        <v>0.47466666666666602</v>
+      </c>
+      <c r="Q78">
+        <v>0.490671641791044</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>43</v>
+      </c>
+      <c r="B79" t="s">
+        <v>44</v>
+      </c>
+      <c r="C79">
+        <v>0.44810247421264598</v>
+      </c>
+      <c r="D79" t="s">
+        <v>45</v>
+      </c>
+      <c r="E79" t="s">
+        <v>43</v>
+      </c>
+      <c r="I79" t="s">
+        <v>43</v>
+      </c>
+      <c r="J79" t="s">
+        <v>44</v>
+      </c>
+      <c r="K79">
+        <v>0.111025094985961</v>
+      </c>
+      <c r="L79" t="s">
+        <v>45</v>
+      </c>
+      <c r="M79" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>43</v>
+      </c>
+      <c r="R79" t="s">
+        <v>44</v>
+      </c>
+      <c r="S79">
+        <v>0.34307789802551197</v>
+      </c>
+      <c r="T79" t="s">
+        <v>45</v>
+      </c>
+      <c r="U79" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80">
+        <v>292</v>
+      </c>
+      <c r="I80" t="s">
+        <v>42</v>
+      </c>
+      <c r="J80">
+        <v>87</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>42</v>
+      </c>
+      <c r="R80">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>37</v>
+      </c>
+      <c r="B81">
+        <v>518</v>
+      </c>
+      <c r="I81" t="s">
+        <v>37</v>
+      </c>
+      <c r="J81">
+        <v>127</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>37</v>
+      </c>
+      <c r="R81">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>36</v>
+      </c>
+      <c r="B82">
+        <v>637</v>
+      </c>
+      <c r="I82" t="s">
+        <v>36</v>
+      </c>
+      <c r="J82">
+        <v>161</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>36</v>
+      </c>
+      <c r="R82">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>32</v>
+      </c>
+      <c r="C85" t="s">
+        <v>33</v>
+      </c>
+      <c r="D85" t="s">
+        <v>34</v>
+      </c>
+      <c r="E85" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>36</v>
+      </c>
+      <c r="C87">
+        <v>0.89</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>0.94</v>
+      </c>
+      <c r="F87">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>37</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" t="s">
+        <v>39</v>
+      </c>
+      <c r="D90">
+        <v>0.89</v>
+      </c>
+      <c r="E90">
+        <v>0.89</v>
+      </c>
+      <c r="F90">
+        <v>0.89</v>
+      </c>
+      <c r="G90">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>40</v>
+      </c>
+      <c r="C91" t="s">
+        <v>39</v>
+      </c>
+      <c r="D91">
+        <v>0.45</v>
+      </c>
+      <c r="E91">
+        <v>0.5</v>
+      </c>
+      <c r="F91">
+        <v>0.47</v>
+      </c>
+      <c r="G91">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>41</v>
+      </c>
+      <c r="B92" t="s">
+        <v>39</v>
+      </c>
+      <c r="C92">
+        <v>0.8</v>
+      </c>
+      <c r="D92">
+        <v>0.89</v>
+      </c>
+      <c r="E92">
+        <v>0.84</v>
+      </c>
+      <c r="F92">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>32</v>
+      </c>
+      <c r="C94" t="s">
+        <v>33</v>
+      </c>
+      <c r="D94" t="s">
+        <v>34</v>
+      </c>
+      <c r="E94" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>36</v>
+      </c>
+      <c r="C96">
+        <v>0.89</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>0.94</v>
+      </c>
+      <c r="F96">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>37</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>38</v>
+      </c>
+      <c r="C99" t="s">
+        <v>39</v>
+      </c>
+      <c r="D99">
+        <v>0.89</v>
+      </c>
+      <c r="E99">
+        <v>0.89</v>
+      </c>
+      <c r="F99">
+        <v>0.89</v>
+      </c>
+      <c r="G99">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>40</v>
+      </c>
+      <c r="C100" t="s">
+        <v>39</v>
+      </c>
+      <c r="D100">
+        <v>0.45</v>
+      </c>
+      <c r="E100">
+        <v>0.5</v>
+      </c>
+      <c r="F100">
+        <v>0.47</v>
+      </c>
+      <c r="G100">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>41</v>
+      </c>
+      <c r="B101" t="s">
+        <v>39</v>
+      </c>
+      <c r="C101">
+        <v>0.8</v>
+      </c>
+      <c r="D101">
+        <v>0.89</v>
+      </c>
+      <c r="E101">
+        <v>0.84</v>
+      </c>
+      <c r="F101">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103">
+        <v>200</v>
+      </c>
+      <c r="C103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D103">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="E103">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="F103">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="G103">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="H103">
+        <v>0.5</v>
+      </c>
+      <c r="I103">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="J103">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="K103">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="L103">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="M103">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>8</v>
+      </c>
+      <c r="B104">
+        <v>200</v>
+      </c>
+      <c r="C104" t="s">
+        <v>15</v>
+      </c>
+      <c r="D104">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="E104">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="F104">
+        <v>0.8</v>
+      </c>
+      <c r="G104">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="H104">
+        <v>0.5</v>
+      </c>
+      <c r="I104">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="J104">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="K104">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="L104">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="M104">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>32</v>
+      </c>
+      <c r="C107" t="s">
+        <v>33</v>
+      </c>
+      <c r="D107" t="s">
+        <v>34</v>
+      </c>
+      <c r="E107" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>36</v>
+      </c>
+      <c r="C109">
+        <v>0.92</v>
+      </c>
+      <c r="D109">
+        <v>0.97</v>
+      </c>
+      <c r="E109">
+        <v>0.95</v>
+      </c>
+      <c r="F109">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>37</v>
+      </c>
+      <c r="C110">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D110">
+        <v>0.3</v>
+      </c>
+      <c r="E110">
+        <v>0.39</v>
+      </c>
+      <c r="F110">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>38</v>
+      </c>
+      <c r="C112" t="s">
+        <v>39</v>
+      </c>
+      <c r="D112">
+        <v>0.9</v>
+      </c>
+      <c r="E112">
+        <v>0.9</v>
+      </c>
+      <c r="F112">
+        <v>0.9</v>
+      </c>
+      <c r="G112">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>40</v>
+      </c>
+      <c r="C113" t="s">
+        <v>39</v>
+      </c>
+      <c r="D113">
+        <v>0.75</v>
+      </c>
+      <c r="E113">
+        <v>0.64</v>
+      </c>
+      <c r="F113">
+        <v>0.67</v>
+      </c>
+      <c r="G113">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>41</v>
+      </c>
+      <c r="B114" t="s">
+        <v>39</v>
+      </c>
+      <c r="C114">
+        <v>0.88</v>
+      </c>
+      <c r="D114">
+        <v>0.9</v>
+      </c>
+      <c r="E114">
+        <v>0.89</v>
+      </c>
+      <c r="F114">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>32</v>
+      </c>
+      <c r="C116" t="s">
+        <v>33</v>
+      </c>
+      <c r="D116" t="s">
+        <v>34</v>
+      </c>
+      <c r="E116" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>36</v>
+      </c>
+      <c r="C118">
+        <v>0.95</v>
+      </c>
+      <c r="D118">
+        <v>0.97</v>
+      </c>
+      <c r="E118">
+        <v>0.96</v>
+      </c>
+      <c r="F118">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>37</v>
+      </c>
+      <c r="C119">
+        <v>0.69</v>
+      </c>
+      <c r="D119">
+        <v>0.53</v>
+      </c>
+      <c r="E119">
+        <v>0.6</v>
+      </c>
+      <c r="F119">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>38</v>
+      </c>
+      <c r="C121" t="s">
+        <v>39</v>
+      </c>
+      <c r="D121">
+        <v>0.93</v>
+      </c>
+      <c r="E121">
+        <v>0.93</v>
+      </c>
+      <c r="F121">
+        <v>0.93</v>
+      </c>
+      <c r="G121">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>40</v>
+      </c>
+      <c r="C122" t="s">
+        <v>39</v>
+      </c>
+      <c r="D122">
+        <v>0.82</v>
+      </c>
+      <c r="E122">
+        <v>0.75</v>
+      </c>
+      <c r="F122">
+        <v>0.78</v>
+      </c>
+      <c r="G122">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>41</v>
+      </c>
+      <c r="B123" t="s">
+        <v>39</v>
+      </c>
+      <c r="C123">
+        <v>0.92</v>
+      </c>
+      <c r="D123">
+        <v>0.93</v>
+      </c>
+      <c r="E123">
+        <v>0.92</v>
+      </c>
+      <c r="F123">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>10</v>
+      </c>
+      <c r="B125">
+        <v>200</v>
+      </c>
+      <c r="C125" t="s">
+        <v>14</v>
+      </c>
+      <c r="D125">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="E125">
+        <v>0.746</v>
+      </c>
+      <c r="F125">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="G125">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="H125">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="I125">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="J125">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="K125">
+        <v>0.67</v>
+      </c>
+      <c r="L125">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="M125">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>10</v>
+      </c>
+      <c r="B126">
+        <v>200</v>
+      </c>
+      <c r="C126" t="s">
+        <v>15</v>
+      </c>
+      <c r="D126">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="E126">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="F126">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="G126">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="H126">
+        <v>0.751</v>
+      </c>
+      <c r="I126">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="J126">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="K126">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="L126">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="M126">
+        <v>7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>32</v>
+      </c>
+      <c r="C129" t="s">
+        <v>33</v>
+      </c>
+      <c r="D129" t="s">
+        <v>34</v>
+      </c>
+      <c r="E129" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>36</v>
+      </c>
+      <c r="C131">
+        <v>0.92</v>
+      </c>
+      <c r="D131">
+        <v>0.96</v>
+      </c>
+      <c r="E131">
+        <v>0.94</v>
+      </c>
+      <c r="F131">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>37</v>
+      </c>
+      <c r="C132">
+        <v>0.5</v>
+      </c>
+      <c r="D132">
+        <v>0.3</v>
+      </c>
+      <c r="E132">
+        <v>0.37</v>
+      </c>
+      <c r="F132">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>38</v>
+      </c>
+      <c r="C134" t="s">
+        <v>39</v>
+      </c>
+      <c r="D134">
+        <v>0.89</v>
+      </c>
+      <c r="E134">
+        <v>0.89</v>
+      </c>
+      <c r="F134">
+        <v>0.89</v>
+      </c>
+      <c r="G134">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>40</v>
+      </c>
+      <c r="C135" t="s">
+        <v>39</v>
+      </c>
+      <c r="D135">
+        <v>0.71</v>
+      </c>
+      <c r="E135">
+        <v>0.63</v>
+      </c>
+      <c r="F135">
+        <v>0.66</v>
+      </c>
+      <c r="G135">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>41</v>
+      </c>
+      <c r="B136" t="s">
+        <v>39</v>
+      </c>
+      <c r="C136">
+        <v>0.88</v>
+      </c>
+      <c r="D136">
+        <v>0.89</v>
+      </c>
+      <c r="E136">
+        <v>0.88</v>
+      </c>
+      <c r="F136">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>32</v>
+      </c>
+      <c r="C138" t="s">
+        <v>33</v>
+      </c>
+      <c r="D138" t="s">
+        <v>34</v>
+      </c>
+      <c r="E138" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>36</v>
+      </c>
+      <c r="C140">
+        <v>0.95</v>
+      </c>
+      <c r="D140">
+        <v>0.98</v>
+      </c>
+      <c r="E140">
+        <v>0.96</v>
+      </c>
+      <c r="F140">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>37</v>
+      </c>
+      <c r="C141">
+        <v>0.73</v>
+      </c>
+      <c r="D141">
+        <v>0.54</v>
+      </c>
+      <c r="E141">
+        <v>0.62</v>
+      </c>
+      <c r="F141">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>38</v>
+      </c>
+      <c r="C143" t="s">
+        <v>39</v>
+      </c>
+      <c r="D143">
+        <v>0.93</v>
+      </c>
+      <c r="E143">
+        <v>0.93</v>
+      </c>
+      <c r="F143">
+        <v>0.93</v>
+      </c>
+      <c r="G143">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>40</v>
+      </c>
+      <c r="C144" t="s">
+        <v>39</v>
+      </c>
+      <c r="D144">
+        <v>0.84</v>
+      </c>
+      <c r="E144">
+        <v>0.76</v>
+      </c>
+      <c r="F144">
+        <v>0.79</v>
+      </c>
+      <c r="G144">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>41</v>
+      </c>
+      <c r="B145" t="s">
+        <v>39</v>
+      </c>
+      <c r="C145">
+        <v>0.93</v>
+      </c>
+      <c r="D145">
+        <v>0.93</v>
+      </c>
+      <c r="E145">
+        <v>0.93</v>
+      </c>
+      <c r="F145">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>12</v>
+      </c>
+      <c r="B147">
+        <v>200</v>
+      </c>
+      <c r="C147" t="s">
+        <v>14</v>
+      </c>
+      <c r="D147">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="E147">
+        <v>0.71</v>
+      </c>
+      <c r="F147">
+        <v>0.875</v>
+      </c>
+      <c r="G147">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="H147">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="I147">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="J147">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="K147">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="L147">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="M147">
+        <v>2.35E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>12</v>
+      </c>
+      <c r="B148">
+        <v>200</v>
+      </c>
+      <c r="C148" t="s">
+        <v>15</v>
+      </c>
+      <c r="D148">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="E148">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="F148">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="G148">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="H148">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="I148">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="J148">
+        <v>0.93100000000000005</v>
+      </c>
+      <c r="K148">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="L148">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="M148">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
uncommented report statement to gen data
</commit_message>
<xml_diff>
--- a/data_dump.xlsx
+++ b/data_dump.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\King\cs9414-opinion-mining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF0CF5E-542B-44A0-8F35-89919D8BF2CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF31D057-81E6-466F-9167-190281DDCD38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
+    <workbookView xWindow="4020" yWindow="2370" windowWidth="20310" windowHeight="11505" activeTab="2" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Q5" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Q5'!$O$44:$O$64</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$M$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="47">
   <si>
     <t>Classifier</t>
   </si>
@@ -152,18 +153,6 @@
     <t>positive</t>
   </si>
   <si>
-    <t>micro</t>
-  </si>
-  <si>
-    <t>avg</t>
-  </si>
-  <si>
-    <t>macro</t>
-  </si>
-  <si>
-    <t>weighted</t>
-  </si>
-  <si>
     <t>neutral</t>
   </si>
   <si>
@@ -174,6 +163,21 @@
   </si>
   <si>
     <t>seconds</t>
+  </si>
+  <si>
+    <t>micro avg</t>
+  </si>
+  <si>
+    <t>macro avg</t>
+  </si>
+  <si>
+    <t>weighted avg</t>
+  </si>
+  <si>
+    <t>DT_sentiment    200     test    0.672   0.452   0.617   0.672   0.410   0.672   0.672   0.405   0.634   0.0210</t>
+  </si>
+  <si>
+    <t>DT_sentiment    200     train   0.699   0.577   0.667   0.699   0.469   0.699   0.699   0.482   0.667   0.0360</t>
   </si>
 </sst>
 </file>
@@ -3194,71 +3198,116 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96611E49-C074-44E2-ADBF-AAB639D2C6AE}">
-  <dimension ref="A1:W148"/>
+  <dimension ref="A2:V148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="M135" sqref="M135"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>36</v>
       </c>
+      <c r="C3">
+        <v>0.91</v>
+      </c>
       <c r="D3">
-        <v>0.91</v>
+        <v>0.99</v>
       </c>
       <c r="E3">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="F3">
-        <v>0.95</v>
-      </c>
-      <c r="G3">
         <v>335</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>37</v>
       </c>
+      <c r="C4">
+        <v>0.62</v>
+      </c>
       <c r="D4">
-        <v>0.62</v>
+        <v>0.2</v>
       </c>
       <c r="E4">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="F4">
-        <v>0.3</v>
-      </c>
-      <c r="G4">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4">
+        <v>0.74</v>
+      </c>
+      <c r="R4">
+        <v>0.88</v>
+      </c>
+      <c r="S4">
+        <v>0.8</v>
+      </c>
+      <c r="T4">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q5">
+        <v>0.41</v>
+      </c>
+      <c r="R5">
+        <v>0.33</v>
+      </c>
+      <c r="S5">
+        <v>0.37</v>
+      </c>
+      <c r="T5">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C6">
+        <v>0.9</v>
       </c>
       <c r="D6">
         <v>0.9</v>
@@ -3267,106 +3316,218 @@
         <v>0.9</v>
       </c>
       <c r="F6">
+        <v>375</v>
+      </c>
+      <c r="P6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6">
+        <v>0.2</v>
+      </c>
+      <c r="R6">
+        <v>0.03</v>
+      </c>
+      <c r="S6">
+        <v>0.04</v>
+      </c>
+      <c r="T6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7">
+        <v>0.76</v>
+      </c>
+      <c r="D7">
+        <v>0.59</v>
+      </c>
+      <c r="E7">
+        <v>0.62</v>
+      </c>
+      <c r="F7">
+        <v>375</v>
+      </c>
+      <c r="P7" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7">
+        <v>0.67</v>
+      </c>
+      <c r="R7">
+        <v>0.67</v>
+      </c>
+      <c r="S7">
+        <v>0.67</v>
+      </c>
+      <c r="T7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8">
+        <v>0.88</v>
+      </c>
+      <c r="D8">
         <v>0.9</v>
       </c>
-      <c r="G6">
+      <c r="E8">
+        <v>0.88</v>
+      </c>
+      <c r="F8">
         <v>375</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7">
-        <v>0.76</v>
-      </c>
-      <c r="E7">
-        <v>0.59</v>
-      </c>
-      <c r="F7">
+      <c r="P8" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q8">
+        <v>0.45</v>
+      </c>
+      <c r="R8">
+        <v>0.41</v>
+      </c>
+      <c r="S8">
+        <v>0.4</v>
+      </c>
+      <c r="T8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="P9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q9">
         <v>0.62</v>
       </c>
-      <c r="G7">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8">
-        <v>0.88</v>
-      </c>
-      <c r="E8">
-        <v>0.9</v>
-      </c>
-      <c r="F8">
-        <v>0.88</v>
-      </c>
-      <c r="G8">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="R9">
+        <v>0.67</v>
+      </c>
+      <c r="S9">
+        <v>0.63</v>
+      </c>
+      <c r="T9">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="Q11" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11" t="s">
+        <v>33</v>
+      </c>
+      <c r="S11" t="s">
+        <v>34</v>
+      </c>
+      <c r="T11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>36</v>
       </c>
+      <c r="C12">
+        <v>0.92</v>
+      </c>
       <c r="D12">
-        <v>0.92</v>
+        <v>0.98</v>
       </c>
       <c r="E12">
-        <v>0.98</v>
+        <v>0.95</v>
       </c>
       <c r="F12">
-        <v>0.95</v>
-      </c>
-      <c r="G12">
         <v>959</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P12" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q12">
+        <v>0.74</v>
+      </c>
+      <c r="R12">
+        <v>0.9</v>
+      </c>
+      <c r="S12">
+        <v>0.81</v>
+      </c>
+      <c r="T12">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>37</v>
       </c>
+      <c r="C13">
+        <v>0.65</v>
+      </c>
       <c r="D13">
-        <v>0.65</v>
+        <v>0.25</v>
       </c>
       <c r="E13">
-        <v>0.25</v>
+        <v>0.36</v>
       </c>
       <c r="F13">
-        <v>0.36</v>
-      </c>
-      <c r="G13">
         <v>113</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="P13" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="R13">
+        <v>0.41</v>
+      </c>
+      <c r="S13">
+        <v>0.48</v>
+      </c>
+      <c r="T13">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="P14" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q14">
+        <v>0.42</v>
+      </c>
+      <c r="R14">
+        <v>0.1</v>
+      </c>
+      <c r="S14">
+        <v>0.16</v>
+      </c>
+      <c r="T14">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C15">
+        <v>0.91</v>
       </c>
       <c r="D15">
         <v>0.91</v>
@@ -3375,53 +3536,89 @@
         <v>0.91</v>
       </c>
       <c r="F15">
+        <v>1072</v>
+      </c>
+      <c r="P15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q15">
+        <v>0.7</v>
+      </c>
+      <c r="R15">
+        <v>0.7</v>
+      </c>
+      <c r="S15">
+        <v>0.7</v>
+      </c>
+      <c r="T15">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16">
+        <v>0.78</v>
+      </c>
+      <c r="D16">
+        <v>0.62</v>
+      </c>
+      <c r="E16">
+        <v>0.65</v>
+      </c>
+      <c r="F16">
+        <v>1072</v>
+      </c>
+      <c r="P16" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q16">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="R16">
+        <v>0.47</v>
+      </c>
+      <c r="S16">
+        <v>0.48</v>
+      </c>
+      <c r="T16">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17">
+        <v>0.89</v>
+      </c>
+      <c r="D17">
         <v>0.91</v>
       </c>
-      <c r="G15">
+      <c r="E17">
+        <v>0.89</v>
+      </c>
+      <c r="F17">
         <v>1072</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16">
-        <v>0.78</v>
-      </c>
-      <c r="E16">
-        <v>0.62</v>
-      </c>
-      <c r="F16">
-        <v>0.65</v>
-      </c>
-      <c r="G16">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17">
-        <v>0.89</v>
-      </c>
-      <c r="E17">
-        <v>0.91</v>
-      </c>
-      <c r="F17">
-        <v>0.89</v>
-      </c>
-      <c r="G17">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q17">
+        <v>0.67</v>
+      </c>
+      <c r="R17">
+        <v>0.7</v>
+      </c>
+      <c r="S17">
+        <v>0.67</v>
+      </c>
+      <c r="T17">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -3462,7 +3659,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -3503,60 +3700,114 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>32</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E24" t="s">
         <v>34</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>36</v>
       </c>
+      <c r="C25">
+        <v>0.93</v>
+      </c>
       <c r="D25">
-        <v>0.93</v>
+        <v>0.97</v>
       </c>
       <c r="E25">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="F25">
-        <v>0.95</v>
-      </c>
-      <c r="G25">
         <v>335</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q25" t="s">
+        <v>32</v>
+      </c>
+      <c r="R25" t="s">
+        <v>33</v>
+      </c>
+      <c r="S25" t="s">
+        <v>34</v>
+      </c>
+      <c r="T25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>37</v>
       </c>
+      <c r="C26">
+        <v>0.56000000000000005</v>
+      </c>
       <c r="D26">
-        <v>0.56000000000000005</v>
+        <v>0.35</v>
       </c>
       <c r="E26">
-        <v>0.35</v>
+        <v>0.43</v>
       </c>
       <c r="F26">
-        <v>0.43</v>
-      </c>
-      <c r="G26">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P26" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q26">
+        <v>0.79</v>
+      </c>
+      <c r="R26">
+        <v>0.86</v>
+      </c>
+      <c r="S26">
+        <v>0.82</v>
+      </c>
+      <c r="T26">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q27">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="R27">
+        <v>0.53</v>
+      </c>
+      <c r="S27">
+        <v>0.54</v>
+      </c>
+      <c r="T27">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C28">
+        <v>0.9</v>
       </c>
       <c r="D28">
         <v>0.9</v>
@@ -3565,106 +3816,218 @@
         <v>0.9</v>
       </c>
       <c r="F28">
+        <v>375</v>
+      </c>
+      <c r="P28" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q28">
+        <v>0.5</v>
+      </c>
+      <c r="R28">
+        <v>0.23</v>
+      </c>
+      <c r="S28">
+        <v>0.31</v>
+      </c>
+      <c r="T28">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29">
+        <v>0.74</v>
+      </c>
+      <c r="D29">
+        <v>0.66</v>
+      </c>
+      <c r="E29">
+        <v>0.69</v>
+      </c>
+      <c r="F29">
+        <v>375</v>
+      </c>
+      <c r="P29" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q29">
+        <v>0.72</v>
+      </c>
+      <c r="R29">
+        <v>0.72</v>
+      </c>
+      <c r="S29">
+        <v>0.72</v>
+      </c>
+      <c r="T29">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30">
+        <v>0.89</v>
+      </c>
+      <c r="D30">
         <v>0.9</v>
       </c>
-      <c r="G28">
+      <c r="E30">
+        <v>0.89</v>
+      </c>
+      <c r="F30">
         <v>375</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29">
-        <v>0.74</v>
-      </c>
-      <c r="E29">
-        <v>0.66</v>
-      </c>
-      <c r="F29">
-        <v>0.69</v>
-      </c>
-      <c r="G29">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30">
-        <v>0.89</v>
-      </c>
-      <c r="E30">
-        <v>0.9</v>
-      </c>
-      <c r="F30">
-        <v>0.89</v>
-      </c>
-      <c r="G30">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="P30" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q30">
+        <v>0.62</v>
+      </c>
+      <c r="R30">
+        <v>0.54</v>
+      </c>
+      <c r="S30">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="T30">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P31" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q31">
+        <v>0.71</v>
+      </c>
+      <c r="R31">
+        <v>0.72</v>
+      </c>
+      <c r="S31">
+        <v>0.71</v>
+      </c>
+      <c r="T31">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>32</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D33" t="s">
         <v>33</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E33" t="s">
         <v>34</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q33" t="s">
+        <v>32</v>
+      </c>
+      <c r="R33" t="s">
+        <v>33</v>
+      </c>
+      <c r="S33" t="s">
+        <v>34</v>
+      </c>
+      <c r="T33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>36</v>
       </c>
+      <c r="C34">
+        <v>0.94</v>
+      </c>
       <c r="D34">
-        <v>0.94</v>
+        <v>0.96</v>
       </c>
       <c r="E34">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="F34">
-        <v>0.95</v>
-      </c>
-      <c r="G34">
         <v>959</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P34" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q34">
+        <v>0.8</v>
+      </c>
+      <c r="R34">
+        <v>0.86</v>
+      </c>
+      <c r="S34">
+        <v>0.83</v>
+      </c>
+      <c r="T34">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>37</v>
       </c>
+      <c r="C35">
+        <v>0.61</v>
+      </c>
       <c r="D35">
-        <v>0.61</v>
+        <v>0.51</v>
       </c>
       <c r="E35">
-        <v>0.51</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F35">
+        <v>113</v>
+      </c>
+      <c r="P35" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q35">
+        <v>0.66</v>
+      </c>
+      <c r="R35">
+        <v>0.59</v>
+      </c>
+      <c r="S35">
+        <v>0.62</v>
+      </c>
+      <c r="T35">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P36" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q36">
+        <v>0.65</v>
+      </c>
+      <c r="R36">
+        <v>0.49</v>
+      </c>
+      <c r="S36">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G35">
+      <c r="T36">
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C37">
+        <v>0.91</v>
       </c>
       <c r="D37">
         <v>0.91</v>
@@ -3673,38 +4036,62 @@
         <v>0.91</v>
       </c>
       <c r="F37">
+        <v>1072</v>
+      </c>
+      <c r="P37" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q37">
+        <v>0.76</v>
+      </c>
+      <c r="R37">
+        <v>0.76</v>
+      </c>
+      <c r="S37">
+        <v>0.76</v>
+      </c>
+      <c r="T37">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38">
+        <v>0.78</v>
+      </c>
+      <c r="D38">
+        <v>0.74</v>
+      </c>
+      <c r="E38">
+        <v>0.76</v>
+      </c>
+      <c r="F38">
+        <v>1072</v>
+      </c>
+      <c r="P38" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q38">
+        <v>0.7</v>
+      </c>
+      <c r="R38">
+        <v>0.65</v>
+      </c>
+      <c r="S38">
+        <v>0.67</v>
+      </c>
+      <c r="T38">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39">
         <v>0.91</v>
-      </c>
-      <c r="G37">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38">
-        <v>0.78</v>
-      </c>
-      <c r="E38">
-        <v>0.74</v>
-      </c>
-      <c r="F38">
-        <v>0.76</v>
-      </c>
-      <c r="G38">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" t="s">
-        <v>39</v>
       </c>
       <c r="D39">
         <v>0.91</v>
@@ -3713,13 +4100,25 @@
         <v>0.91</v>
       </c>
       <c r="F39">
-        <v>0.91</v>
-      </c>
-      <c r="G39">
         <v>1072</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P39" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q39">
+        <v>0.75</v>
+      </c>
+      <c r="R39">
+        <v>0.76</v>
+      </c>
+      <c r="S39">
+        <v>0.75</v>
+      </c>
+      <c r="T39">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -3760,7 +4159,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -3801,60 +4200,119 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
         <v>32</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D46" t="s">
         <v>33</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E46" t="s">
         <v>34</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F46" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="Q46" t="s">
+        <v>32</v>
+      </c>
+      <c r="R46" t="s">
+        <v>33</v>
+      </c>
+      <c r="S46" t="s">
+        <v>34</v>
+      </c>
+      <c r="T46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>36</v>
       </c>
+      <c r="C47">
+        <v>0.92</v>
+      </c>
       <c r="D47">
-        <v>0.92</v>
+        <v>0.97</v>
       </c>
       <c r="E47">
-        <v>0.97</v>
+        <v>0.94</v>
       </c>
       <c r="F47">
-        <v>0.94</v>
-      </c>
-      <c r="G47">
         <v>335</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P47" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q47">
+        <v>0.79</v>
+      </c>
+      <c r="R47">
+        <v>0.88</v>
+      </c>
+      <c r="S47">
+        <v>0.83</v>
+      </c>
+      <c r="T47">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>37</v>
       </c>
+      <c r="C48">
+        <v>0.52</v>
+      </c>
       <c r="D48">
+        <v>0.3</v>
+      </c>
+      <c r="E48">
+        <v>0.38</v>
+      </c>
+      <c r="F48">
+        <v>40</v>
+      </c>
+      <c r="P48" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q48">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="R48">
         <v>0.52</v>
       </c>
-      <c r="E48">
+      <c r="S48">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="T48">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P49" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q49">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="R49">
+        <v>0.2</v>
+      </c>
+      <c r="S49">
         <v>0.3</v>
       </c>
-      <c r="F48">
-        <v>0.38</v>
-      </c>
-      <c r="G48">
+      <c r="T49">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>38</v>
-      </c>
-      <c r="C50" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C50">
+        <v>0.9</v>
       </c>
       <c r="D50">
         <v>0.9</v>
@@ -3863,106 +4321,218 @@
         <v>0.9</v>
       </c>
       <c r="F50">
+        <v>375</v>
+      </c>
+      <c r="P50" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q50">
+        <v>0.74</v>
+      </c>
+      <c r="R50">
+        <v>0.74</v>
+      </c>
+      <c r="S50">
+        <v>0.74</v>
+      </c>
+      <c r="T50">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>43</v>
+      </c>
+      <c r="C51">
+        <v>0.72</v>
+      </c>
+      <c r="D51">
+        <v>0.63</v>
+      </c>
+      <c r="E51">
+        <v>0.66</v>
+      </c>
+      <c r="F51">
+        <v>375</v>
+      </c>
+      <c r="P51" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q51">
+        <v>0.65</v>
+      </c>
+      <c r="R51">
+        <v>0.53</v>
+      </c>
+      <c r="S51">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="T51">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52">
+        <v>0.88</v>
+      </c>
+      <c r="D52">
         <v>0.9</v>
       </c>
-      <c r="G50">
+      <c r="E52">
+        <v>0.88</v>
+      </c>
+      <c r="F52">
         <v>375</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" t="s">
-        <v>39</v>
-      </c>
-      <c r="D51">
+      <c r="P52" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q52">
         <v>0.72</v>
       </c>
-      <c r="E51">
-        <v>0.63</v>
-      </c>
-      <c r="F51">
-        <v>0.66</v>
-      </c>
-      <c r="G51">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>41</v>
-      </c>
-      <c r="B52" t="s">
-        <v>39</v>
-      </c>
-      <c r="D52">
-        <v>0.88</v>
-      </c>
-      <c r="E52">
-        <v>0.9</v>
-      </c>
-      <c r="F52">
-        <v>0.88</v>
-      </c>
-      <c r="G52">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="R52">
+        <v>0.74</v>
+      </c>
+      <c r="S52">
+        <v>0.72</v>
+      </c>
+      <c r="T52">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Q54" t="s">
         <v>32</v>
       </c>
-      <c r="C54" t="s">
+      <c r="R54" t="s">
         <v>33</v>
       </c>
-      <c r="D54" t="s">
+      <c r="S54" t="s">
         <v>34</v>
       </c>
-      <c r="E54" t="s">
+      <c r="T54" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>32</v>
+      </c>
+      <c r="D55" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" t="s">
+        <v>34</v>
+      </c>
+      <c r="F55" t="s">
+        <v>35</v>
+      </c>
+      <c r="P55" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q55">
+        <v>0.8</v>
+      </c>
+      <c r="R55">
+        <v>0.87</v>
+      </c>
+      <c r="S55">
+        <v>0.83</v>
+      </c>
+      <c r="T55">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>36</v>
       </c>
+      <c r="C56">
+        <v>0.94</v>
+      </c>
       <c r="D56">
-        <v>0.94</v>
+        <v>0.97</v>
       </c>
       <c r="E56">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="F56">
-        <v>0.95</v>
-      </c>
-      <c r="G56">
         <v>959</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P56" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q56">
+        <v>0.66</v>
+      </c>
+      <c r="R56">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="S56">
+        <v>0.62</v>
+      </c>
+      <c r="T56">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>37</v>
       </c>
+      <c r="C57">
+        <v>0.64</v>
+      </c>
       <c r="D57">
+        <v>0.5</v>
+      </c>
+      <c r="E57">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F57">
+        <v>113</v>
+      </c>
+      <c r="P57" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q57">
         <v>0.64</v>
       </c>
-      <c r="E57">
-        <v>0.5</v>
-      </c>
-      <c r="F57">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="G57">
+      <c r="R57">
+        <v>0.43</v>
+      </c>
+      <c r="S57">
+        <v>0.52</v>
+      </c>
+      <c r="T57">
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P58" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q58">
+        <v>0.76</v>
+      </c>
+      <c r="R58">
+        <v>0.76</v>
+      </c>
+      <c r="S58">
+        <v>0.76</v>
+      </c>
+      <c r="T58">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>38</v>
-      </c>
-      <c r="C59" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C59">
+        <v>0.92</v>
       </c>
       <c r="D59">
         <v>0.92</v>
@@ -3971,53 +4541,74 @@
         <v>0.92</v>
       </c>
       <c r="F59">
+        <v>1072</v>
+      </c>
+      <c r="P59" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q59">
+        <v>0.7</v>
+      </c>
+      <c r="R59">
+        <v>0.63</v>
+      </c>
+      <c r="S59">
+        <v>0.66</v>
+      </c>
+      <c r="T59">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60">
+        <v>0.79</v>
+      </c>
+      <c r="D60">
+        <v>0.74</v>
+      </c>
+      <c r="E60">
+        <v>0.76</v>
+      </c>
+      <c r="F60">
+        <v>1072</v>
+      </c>
+      <c r="P60" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q60">
+        <v>0.75</v>
+      </c>
+      <c r="R60">
+        <v>0.76</v>
+      </c>
+      <c r="S60">
+        <v>0.75</v>
+      </c>
+      <c r="T60">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61">
+        <v>0.91</v>
+      </c>
+      <c r="D61">
         <v>0.92</v>
       </c>
-      <c r="G59">
+      <c r="E61">
+        <v>0.91</v>
+      </c>
+      <c r="F61">
         <v>1072</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>40</v>
-      </c>
-      <c r="C60" t="s">
-        <v>39</v>
-      </c>
-      <c r="D60">
-        <v>0.79</v>
-      </c>
-      <c r="E60">
-        <v>0.74</v>
-      </c>
-      <c r="F60">
-        <v>0.76</v>
-      </c>
-      <c r="G60">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>41</v>
-      </c>
-      <c r="B61" t="s">
-        <v>39</v>
-      </c>
-      <c r="D61">
-        <v>0.91</v>
-      </c>
-      <c r="E61">
-        <v>0.92</v>
-      </c>
-      <c r="F61">
-        <v>0.91</v>
-      </c>
-      <c r="G61">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -4058,7 +4649,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -4099,45 +4690,73 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="S67" t="s">
         <v>32</v>
       </c>
-      <c r="C68" t="s">
+      <c r="T67" t="s">
         <v>33</v>
       </c>
-      <c r="D68" t="s">
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="R68" t="s">
+        <v>36</v>
+      </c>
+      <c r="S68">
+        <v>0.96</v>
+      </c>
+      <c r="T68">
+        <v>0.48</v>
+      </c>
+      <c r="U68" t="s">
         <v>34</v>
       </c>
-      <c r="E68" t="s">
+      <c r="V68" t="s">
         <v>35</v>
       </c>
-      <c r="J68" t="s">
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
         <v>32</v>
       </c>
-      <c r="K68" t="s">
+      <c r="D69" t="s">
         <v>33</v>
       </c>
-      <c r="L68" t="s">
+      <c r="E69" t="s">
         <v>34</v>
       </c>
-      <c r="M68" t="s">
+      <c r="F69" t="s">
         <v>35</v>
       </c>
-      <c r="R68" t="s">
+      <c r="K69" t="s">
         <v>32</v>
       </c>
-      <c r="S68" t="s">
+      <c r="L69" t="s">
         <v>33</v>
       </c>
-      <c r="T68" t="s">
+      <c r="M69" t="s">
         <v>34</v>
       </c>
-      <c r="U68" t="s">
+      <c r="N69" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R69" t="s">
+        <v>38</v>
+      </c>
+      <c r="S69">
+        <v>0</v>
+      </c>
+      <c r="T69">
+        <v>0</v>
+      </c>
+      <c r="U69">
+        <v>0.64</v>
+      </c>
+      <c r="V69">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>36</v>
       </c>
@@ -4169,24 +4788,24 @@
         <v>335</v>
       </c>
       <c r="R70" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S70">
-        <v>0.96</v>
+        <v>0.18</v>
       </c>
       <c r="T70">
-        <v>0.48</v>
+        <v>0.61</v>
       </c>
       <c r="U70">
-        <v>0.64</v>
+        <v>0</v>
       </c>
       <c r="V70">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -4201,7 +4820,7 @@
         <v>0</v>
       </c>
       <c r="J71" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K71">
         <v>0</v>
@@ -4215,23 +4834,14 @@
       <c r="N71">
         <v>0</v>
       </c>
-      <c r="R71" t="s">
-        <v>42</v>
-      </c>
-      <c r="S71">
-        <v>0</v>
-      </c>
-      <c r="T71">
-        <v>0</v>
-      </c>
       <c r="U71">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="V71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>37</v>
       </c>
@@ -4263,27 +4873,38 @@
         <v>40</v>
       </c>
       <c r="R72" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="S72">
-        <v>0.18</v>
+        <v>0.49</v>
       </c>
       <c r="T72">
-        <v>0.61</v>
-      </c>
-      <c r="U72">
-        <v>0.27</v>
-      </c>
-      <c r="V72">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="R73" t="s">
+        <v>43</v>
+      </c>
+      <c r="S73">
+        <v>0.38</v>
+      </c>
+      <c r="T73">
+        <v>0.36</v>
+      </c>
+      <c r="U73">
+        <v>0.49</v>
+      </c>
+      <c r="V73">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>38</v>
-      </c>
-      <c r="C74" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C74">
+        <v>0.49</v>
       </c>
       <c r="D74">
         <v>0.49</v>
@@ -4292,16 +4913,13 @@
         <v>0.49</v>
       </c>
       <c r="F74">
-        <v>0.49</v>
-      </c>
-      <c r="G74">
         <v>1447</v>
       </c>
       <c r="J74" t="s">
-        <v>38</v>
-      </c>
-      <c r="K74" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="K74">
+        <v>0.47</v>
       </c>
       <c r="L74">
         <v>0.47</v>
@@ -4310,92 +4928,65 @@
         <v>0.47</v>
       </c>
       <c r="N74">
-        <v>0.47</v>
-      </c>
-      <c r="O74">
         <v>375</v>
       </c>
       <c r="R74" t="s">
-        <v>38</v>
-      </c>
-      <c r="S74" t="s">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="S74">
+        <v>0.88</v>
       </c>
       <c r="T74">
         <v>0.49</v>
       </c>
       <c r="U74">
-        <v>0.49</v>
+        <v>0.3</v>
       </c>
       <c r="V74">
-        <v>0.49</v>
-      </c>
-      <c r="W74">
         <v>1072</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>40</v>
-      </c>
-      <c r="C75" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="C75">
+        <v>0.38</v>
       </c>
       <c r="D75">
+        <v>0.36</v>
+      </c>
+      <c r="E75">
+        <v>0.3</v>
+      </c>
+      <c r="F75">
+        <v>1447</v>
+      </c>
+      <c r="J75" t="s">
+        <v>43</v>
+      </c>
+      <c r="K75">
         <v>0.38</v>
       </c>
-      <c r="E75">
+      <c r="L75">
         <v>0.36</v>
       </c>
-      <c r="F75">
-        <v>0.3</v>
-      </c>
-      <c r="G75">
-        <v>1447</v>
-      </c>
-      <c r="J75" t="s">
-        <v>40</v>
-      </c>
-      <c r="K75" t="s">
-        <v>39</v>
-      </c>
-      <c r="L75">
-        <v>0.38</v>
-      </c>
       <c r="M75">
-        <v>0.36</v>
+        <v>0.31</v>
       </c>
       <c r="N75">
-        <v>0.31</v>
-      </c>
-      <c r="O75">
         <v>375</v>
       </c>
-      <c r="R75" t="s">
-        <v>40</v>
-      </c>
-      <c r="S75" t="s">
-        <v>39</v>
-      </c>
-      <c r="T75">
-        <v>0.38</v>
-      </c>
       <c r="U75">
-        <v>0.36</v>
+        <v>0.6</v>
       </c>
       <c r="V75">
-        <v>0.3</v>
-      </c>
-      <c r="W75">
         <v>1072</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>41</v>
-      </c>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C76">
         <v>0.88</v>
@@ -4409,11 +5000,8 @@
       <c r="F76">
         <v>1447</v>
       </c>
-      <c r="I76" t="s">
-        <v>41</v>
-      </c>
       <c r="J76" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="K76">
         <v>0.87</v>
@@ -4427,104 +5015,100 @@
       <c r="N76">
         <v>375</v>
       </c>
-      <c r="Q76" t="s">
+      <c r="Q76">
+        <v>0.490671641791044</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q77" t="s">
+        <v>39</v>
+      </c>
+      <c r="R77" t="s">
+        <v>40</v>
+      </c>
+      <c r="S77">
+        <v>0.34307789802551197</v>
+      </c>
+      <c r="T77" t="s">
         <v>41</v>
       </c>
-      <c r="R76" t="s">
-        <v>39</v>
-      </c>
-      <c r="S76">
-        <v>0.88</v>
-      </c>
-      <c r="T76">
-        <v>0.49</v>
-      </c>
-      <c r="U76">
-        <v>0.6</v>
-      </c>
-      <c r="V76">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0.48652384243261898</v>
       </c>
       <c r="I78">
         <v>0.47466666666666602</v>
       </c>
-      <c r="Q78">
-        <v>0.490671641791044</v>
-      </c>
-    </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Q78" t="s">
+        <v>38</v>
+      </c>
+      <c r="R78">
+        <v>205</v>
+      </c>
+      <c r="U78" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B79" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C79">
         <v>0.44810247421264598</v>
       </c>
       <c r="D79" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E79" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I79" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J79" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="K79">
         <v>0.111025094985961</v>
       </c>
       <c r="L79" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="M79" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q79" t="s">
-        <v>43</v>
-      </c>
-      <c r="R79" t="s">
-        <v>44</v>
-      </c>
-      <c r="S79">
-        <v>0.34307789802551197</v>
-      </c>
-      <c r="T79" t="s">
-        <v>45</v>
-      </c>
-      <c r="U79" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="R79">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B80">
         <v>292</v>
       </c>
       <c r="I80" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="J80">
         <v>87</v>
       </c>
       <c r="Q80" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="R80">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>37</v>
       </c>
@@ -4537,14 +5121,8 @@
       <c r="J81">
         <v>127</v>
       </c>
-      <c r="Q81" t="s">
-        <v>37</v>
-      </c>
-      <c r="R81">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>36</v>
       </c>
@@ -4557,28 +5135,22 @@
       <c r="J82">
         <v>161</v>
       </c>
-      <c r="Q82" t="s">
-        <v>36</v>
-      </c>
-      <c r="R82">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
         <v>32</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D86" t="s">
         <v>33</v>
       </c>
-      <c r="D85" t="s">
+      <c r="E86" t="s">
         <v>34</v>
       </c>
-      <c r="E85" t="s">
+      <c r="F86" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>36</v>
       </c>
@@ -4595,7 +5167,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>37</v>
       </c>
@@ -4612,12 +5184,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>38</v>
-      </c>
-      <c r="C90" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C90">
+        <v>0.89</v>
       </c>
       <c r="D90">
         <v>0.89</v>
@@ -4626,38 +5198,29 @@
         <v>0.89</v>
       </c>
       <c r="F90">
-        <v>0.89</v>
-      </c>
-      <c r="G90">
         <v>375</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>40</v>
-      </c>
-      <c r="C91" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="C91">
+        <v>0.45</v>
       </c>
       <c r="D91">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="E91">
-        <v>0.5</v>
+        <v>0.47</v>
       </c>
       <c r="F91">
-        <v>0.47</v>
-      </c>
-      <c r="G91">
         <v>375</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>41</v>
-      </c>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C92">
         <v>0.8</v>
@@ -4672,21 +5235,21 @@
         <v>375</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
         <v>32</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D95" t="s">
         <v>33</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E95" t="s">
         <v>34</v>
       </c>
-      <c r="E94" t="s">
+      <c r="F95" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>36</v>
       </c>
@@ -4722,10 +5285,10 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>38</v>
-      </c>
-      <c r="C99" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C99">
+        <v>0.89</v>
       </c>
       <c r="D99">
         <v>0.89</v>
@@ -4734,38 +5297,29 @@
         <v>0.89</v>
       </c>
       <c r="F99">
-        <v>0.89</v>
-      </c>
-      <c r="G99">
         <v>1072</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>40</v>
-      </c>
-      <c r="C100" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="C100">
+        <v>0.45</v>
       </c>
       <c r="D100">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="E100">
-        <v>0.5</v>
+        <v>0.47</v>
       </c>
       <c r="F100">
-        <v>0.47</v>
-      </c>
-      <c r="G100">
         <v>1072</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>41</v>
-      </c>
       <c r="B101" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C101">
         <v>0.8</v>
@@ -4862,17 +5416,17 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
         <v>32</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D108" t="s">
         <v>33</v>
       </c>
-      <c r="D107" t="s">
+      <c r="E108" t="s">
         <v>34</v>
       </c>
-      <c r="E107" t="s">
+      <c r="F108" t="s">
         <v>35</v>
       </c>
     </row>
@@ -4912,10 +5466,10 @@
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>38</v>
-      </c>
-      <c r="C112" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C112">
+        <v>0.9</v>
       </c>
       <c r="D112">
         <v>0.9</v>
@@ -4924,38 +5478,29 @@
         <v>0.9</v>
       </c>
       <c r="F112">
-        <v>0.9</v>
-      </c>
-      <c r="G112">
         <v>375</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>40</v>
-      </c>
-      <c r="C113" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="C113">
+        <v>0.75</v>
       </c>
       <c r="D113">
-        <v>0.75</v>
+        <v>0.64</v>
       </c>
       <c r="E113">
-        <v>0.64</v>
+        <v>0.67</v>
       </c>
       <c r="F113">
-        <v>0.67</v>
-      </c>
-      <c r="G113">
         <v>375</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>41</v>
-      </c>
       <c r="B114" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C114">
         <v>0.88</v>
@@ -4970,17 +5515,17 @@
         <v>375</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B116" t="s">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
         <v>32</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D117" t="s">
         <v>33</v>
       </c>
-      <c r="D116" t="s">
+      <c r="E117" t="s">
         <v>34</v>
       </c>
-      <c r="E116" t="s">
+      <c r="F117" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5020,10 +5565,10 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>38</v>
-      </c>
-      <c r="C121" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C121">
+        <v>0.93</v>
       </c>
       <c r="D121">
         <v>0.93</v>
@@ -5032,38 +5577,29 @@
         <v>0.93</v>
       </c>
       <c r="F121">
-        <v>0.93</v>
-      </c>
-      <c r="G121">
         <v>1072</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>40</v>
-      </c>
-      <c r="C122" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="C122">
+        <v>0.82</v>
       </c>
       <c r="D122">
-        <v>0.82</v>
+        <v>0.75</v>
       </c>
       <c r="E122">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
       <c r="F122">
-        <v>0.78</v>
-      </c>
-      <c r="G122">
         <v>1072</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>41</v>
-      </c>
       <c r="B123" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C123">
         <v>0.92</v>
@@ -5160,21 +5696,21 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B129" t="s">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
         <v>32</v>
       </c>
-      <c r="C129" t="s">
+      <c r="D130" t="s">
         <v>33</v>
       </c>
-      <c r="D129" t="s">
+      <c r="E130" t="s">
         <v>34</v>
       </c>
-      <c r="E129" t="s">
+      <c r="F130" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>36</v>
       </c>
@@ -5191,7 +5727,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>37</v>
       </c>
@@ -5208,12 +5744,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>38</v>
-      </c>
-      <c r="C134" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C134">
+        <v>0.89</v>
       </c>
       <c r="D134">
         <v>0.89</v>
@@ -5222,38 +5758,29 @@
         <v>0.89</v>
       </c>
       <c r="F134">
-        <v>0.89</v>
-      </c>
-      <c r="G134">
         <v>375</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>40</v>
-      </c>
-      <c r="C135" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="C135">
+        <v>0.71</v>
       </c>
       <c r="D135">
-        <v>0.71</v>
+        <v>0.63</v>
       </c>
       <c r="E135">
-        <v>0.63</v>
+        <v>0.66</v>
       </c>
       <c r="F135">
-        <v>0.66</v>
-      </c>
-      <c r="G135">
         <v>375</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>41</v>
-      </c>
+    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C136">
         <v>0.88</v>
@@ -5268,21 +5795,21 @@
         <v>375</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B138" t="s">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C139" t="s">
         <v>32</v>
       </c>
-      <c r="C138" t="s">
+      <c r="D139" t="s">
         <v>33</v>
       </c>
-      <c r="D138" t="s">
+      <c r="E139" t="s">
         <v>34</v>
       </c>
-      <c r="E138" t="s">
+      <c r="F139" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>36</v>
       </c>
@@ -5299,7 +5826,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>37</v>
       </c>
@@ -5316,12 +5843,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>38</v>
-      </c>
-      <c r="C143" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C143">
+        <v>0.93</v>
       </c>
       <c r="D143">
         <v>0.93</v>
@@ -5330,38 +5857,29 @@
         <v>0.93</v>
       </c>
       <c r="F143">
-        <v>0.93</v>
-      </c>
-      <c r="G143">
         <v>1072</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>40</v>
-      </c>
-      <c r="C144" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="C144">
+        <v>0.84</v>
       </c>
       <c r="D144">
-        <v>0.84</v>
+        <v>0.76</v>
       </c>
       <c r="E144">
-        <v>0.76</v>
+        <v>0.79</v>
       </c>
       <c r="F144">
-        <v>0.79</v>
-      </c>
-      <c r="G144">
         <v>1072</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>41</v>
-      </c>
       <c r="B145" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C145">
         <v>0.93</v>

</xml_diff>

<commit_message>
Before replacing table 1 in docx
</commit_message>
<xml_diff>
--- a/data_dump.xlsx
+++ b/data_dump.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\King\cs9414-opinion-mining\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doodey\cs9414-opinion-mining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971D25C9-1768-4627-B986-E168E1A2232E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E97F80-C309-4EB0-918F-5D720692D0C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34260" yWindow="1770" windowWidth="20310" windowHeight="11505" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
+    <workbookView xWindow="33915" yWindow="0" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="47">
   <si>
     <t>Classifier</t>
   </si>
@@ -552,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA61A77C-51F7-4D98-BF60-5DD3CA46162A}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -1073,11 +1073,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFAC374A-F1AE-473F-9409-AFFE657A853B}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:AA73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1084,7 @@
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1125,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1137,37 +1136,37 @@
         <v>14</v>
       </c>
       <c r="D2">
-        <v>0.28199999999999997</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="E2">
-        <v>0.17799999999999999</v>
+        <v>0.183</v>
       </c>
       <c r="F2">
-        <v>0.26</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="G2">
-        <v>0.28199999999999997</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="H2">
-        <v>0.161</v>
+        <v>0.152</v>
       </c>
       <c r="I2">
-        <v>0.28199999999999997</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="J2">
-        <v>0.28199999999999997</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="K2">
-        <v>0.16200000000000001</v>
+        <v>0.156</v>
       </c>
       <c r="L2">
-        <v>0.26</v>
+        <v>0.251</v>
       </c>
       <c r="M2">
-        <v>8.9999999999999993E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1178,37 +1177,40 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>0.35099999999999998</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="E3">
-        <v>0.189</v>
+        <v>0.215</v>
       </c>
       <c r="F3">
-        <v>0.30599999999999999</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="G3">
-        <v>0.35099999999999998</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="H3">
-        <v>0.193</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="I3">
-        <v>0.35099999999999998</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="J3">
-        <v>0.35099999999999998</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="K3">
-        <v>0.186</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="L3">
-        <v>0.318</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="M3">
-        <v>8.9999999999999993E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1246,13 +1248,49 @@
         <v>0.27</v>
       </c>
       <c r="M4">
-        <v>2.1000000000000001E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="O4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="P4">
+        <v>200</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R4">
+        <v>0.3</v>
+      </c>
+      <c r="S4">
+        <v>0.187</v>
+      </c>
+      <c r="T4">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="U4">
+        <v>0.3</v>
+      </c>
+      <c r="V4">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="W4">
+        <v>0.3</v>
+      </c>
+      <c r="X4">
+        <v>0.3</v>
+      </c>
+      <c r="Y4">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="Z4">
+        <v>0.27</v>
+      </c>
+      <c r="AA4">
+        <v>4.3499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1290,10 +1328,49 @@
         <v>0.35699999999999998</v>
       </c>
       <c r="M5">
-        <v>2.1999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="O5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P5">
+        <v>200</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>15</v>
+      </c>
+      <c r="R5">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="S5">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="T5">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="U5">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="V5">
+        <v>0.219</v>
+      </c>
+      <c r="W5">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="X5">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="Y5">
+        <v>0.221</v>
+      </c>
+      <c r="Z5">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="AA5">
+        <v>4.4499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1331,10 +1408,10 @@
         <v>0.27</v>
       </c>
       <c r="M6">
-        <v>3.4000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.11600000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1372,10 +1449,10 @@
         <v>0.35699999999999998</v>
       </c>
       <c r="M7">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1413,10 +1490,10 @@
         <v>0.625</v>
       </c>
       <c r="M8">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1454,10 +1531,10 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="M9">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1495,10 +1572,10 @@
         <v>0.63400000000000001</v>
       </c>
       <c r="M10">
-        <v>1.4E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1536,10 +1613,10 @@
         <v>0.66700000000000004</v>
       </c>
       <c r="M11">
-        <v>1.4E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1577,10 +1654,10 @@
         <v>0.63400000000000001</v>
       </c>
       <c r="M12">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>8.9899999999999994E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1618,10 +1695,10 @@
         <v>0.66700000000000004</v>
       </c>
       <c r="M13">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>9.0899999999999995E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1635,16 +1712,16 @@
         <v>0.27</v>
       </c>
       <c r="E14">
-        <v>0.17499999999999999</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="F14">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="G14">
         <v>0.27</v>
       </c>
       <c r="H14">
-        <v>0.15</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="I14">
         <v>0.27</v>
@@ -1653,16 +1730,16 @@
         <v>0.27</v>
       </c>
       <c r="K14">
-        <v>0.155</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="L14">
-        <v>0.25700000000000001</v>
+        <v>0.249</v>
       </c>
       <c r="M14">
-        <v>1.2E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1676,16 +1753,16 @@
         <v>0.40699999999999997</v>
       </c>
       <c r="E15">
-        <v>0.36699999999999999</v>
+        <v>0.38</v>
       </c>
       <c r="F15">
-        <v>0.42099999999999999</v>
+        <v>0.42399999999999999</v>
       </c>
       <c r="G15">
         <v>0.40699999999999997</v>
       </c>
       <c r="H15">
-        <v>0.26300000000000001</v>
+        <v>0.26200000000000001</v>
       </c>
       <c r="I15">
         <v>0.40699999999999997</v>
@@ -1697,13 +1774,13 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="L15">
-        <v>0.39600000000000002</v>
+        <v>0.39400000000000002</v>
       </c>
       <c r="M15">
-        <v>1.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1714,34 +1791,34 @@
         <v>14</v>
       </c>
       <c r="D16">
-        <v>0.32800000000000001</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="E16">
-        <v>0.21099999999999999</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="F16">
-        <v>0.312</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="G16">
-        <v>0.32800000000000001</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="H16">
-        <v>0.18099999999999999</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="I16">
-        <v>0.32800000000000001</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="J16">
-        <v>0.32800000000000001</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="K16">
-        <v>0.184</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="L16">
-        <v>0.30499999999999999</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="M16">
-        <v>1.2999999999999999E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1755,40 +1832,40 @@
         <v>15</v>
       </c>
       <c r="D17">
-        <v>0.50600000000000001</v>
+        <v>0.50900000000000001</v>
       </c>
       <c r="E17">
-        <v>0.47299999999999998</v>
+        <v>0.47199999999999998</v>
       </c>
       <c r="F17">
-        <v>0.52100000000000002</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="G17">
-        <v>0.50600000000000001</v>
+        <v>0.50900000000000001</v>
       </c>
       <c r="H17">
-        <v>0.32600000000000001</v>
+        <v>0.33</v>
       </c>
       <c r="I17">
-        <v>0.50600000000000001</v>
+        <v>0.50900000000000001</v>
       </c>
       <c r="J17">
-        <v>0.50600000000000001</v>
+        <v>0.50900000000000001</v>
       </c>
       <c r="K17">
-        <v>0.35299999999999998</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="L17">
-        <v>0.48899999999999999</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="M17">
-        <v>1.4E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="O17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1799,34 +1876,34 @@
         <v>14</v>
       </c>
       <c r="D18">
-        <v>0.35</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="E18">
-        <v>0.19500000000000001</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="F18">
-        <v>0.33200000000000002</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="G18">
-        <v>0.35</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="H18">
-        <v>0.17599999999999999</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="I18">
-        <v>0.35</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="J18">
-        <v>0.35</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="K18">
-        <v>0.17</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="L18">
-        <v>0.313</v>
+        <v>0.309</v>
       </c>
       <c r="M18">
-        <v>3.2000000000000001E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -1840,37 +1917,37 @@
         <v>15</v>
       </c>
       <c r="D19">
-        <v>0.58099999999999996</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="E19">
-        <v>0.48699999999999999</v>
+        <v>0.48499999999999999</v>
       </c>
       <c r="F19">
-        <v>0.59599999999999997</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="G19">
-        <v>0.58099999999999996</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="H19">
-        <v>0.32400000000000001</v>
+        <v>0.32900000000000001</v>
       </c>
       <c r="I19">
-        <v>0.58099999999999996</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="J19">
-        <v>0.58099999999999996</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="K19">
-        <v>0.33200000000000002</v>
+        <v>0.33700000000000002</v>
       </c>
       <c r="L19">
-        <v>0.54200000000000004</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="M19">
-        <v>3.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1881,34 +1958,34 @@
         <v>14</v>
       </c>
       <c r="D20">
-        <v>0.33600000000000002</v>
+        <v>0.33</v>
       </c>
       <c r="E20">
-        <v>0.20399999999999999</v>
+        <v>0.193</v>
       </c>
       <c r="F20">
-        <v>0.34499999999999997</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="G20">
-        <v>0.33600000000000002</v>
+        <v>0.33</v>
       </c>
       <c r="H20">
-        <v>0.159</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="I20">
-        <v>0.33600000000000002</v>
+        <v>0.33</v>
       </c>
       <c r="J20">
-        <v>0.33600000000000002</v>
+        <v>0.33</v>
       </c>
       <c r="K20">
-        <v>0.156</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="L20">
-        <v>0.29199999999999998</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="M20">
-        <v>2.7E-2</v>
+        <v>5.5E-2</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -1922,37 +1999,37 @@
         <v>15</v>
       </c>
       <c r="D21">
-        <v>0.56899999999999995</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="E21">
-        <v>0.38300000000000001</v>
+        <v>0.378</v>
       </c>
       <c r="F21">
-        <v>0.55300000000000005</v>
+        <v>0.54800000000000004</v>
       </c>
       <c r="G21">
-        <v>0.56899999999999995</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="H21">
-        <v>0.28999999999999998</v>
+        <v>0.29599999999999999</v>
       </c>
       <c r="I21">
-        <v>0.56899999999999995</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="J21">
-        <v>0.56899999999999995</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="K21">
-        <v>0.28699999999999998</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="L21">
-        <v>0.51600000000000001</v>
+        <v>0.52300000000000002</v>
       </c>
       <c r="M21">
-        <v>4.0300000000000002E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>6.7000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1963,37 +2040,37 @@
         <v>14</v>
       </c>
       <c r="D22">
-        <v>0.72</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="E22">
-        <v>0.55400000000000005</v>
+        <v>0.56200000000000006</v>
       </c>
       <c r="F22">
-        <v>0.68799999999999994</v>
+        <v>0.68</v>
       </c>
       <c r="G22">
-        <v>0.72</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="H22">
-        <v>0.48899999999999999</v>
+        <v>0.48499999999999999</v>
       </c>
       <c r="I22">
-        <v>0.72</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="J22">
-        <v>0.72</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="K22">
-        <v>0.505</v>
+        <v>0.504</v>
       </c>
       <c r="L22">
-        <v>0.69499999999999995</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="M22">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2007,16 +2084,16 @@
         <v>0.71899999999999997</v>
       </c>
       <c r="E23">
-        <v>0.64100000000000001</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="F23">
-        <v>0.70099999999999996</v>
+        <v>0.70199999999999996</v>
       </c>
       <c r="G23">
         <v>0.71899999999999997</v>
       </c>
       <c r="H23">
-        <v>0.54700000000000004</v>
+        <v>0.55100000000000005</v>
       </c>
       <c r="I23">
         <v>0.71899999999999997</v>
@@ -2025,16 +2102,16 @@
         <v>0.71899999999999997</v>
       </c>
       <c r="K23">
-        <v>0.57599999999999996</v>
+        <v>0.58099999999999996</v>
       </c>
       <c r="L23">
         <v>0.7</v>
       </c>
       <c r="M23">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2045,40 +2122,40 @@
         <v>14</v>
       </c>
       <c r="D24">
-        <v>0.72399999999999998</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="E24">
-        <v>0.61499999999999999</v>
+        <v>0.56499999999999995</v>
       </c>
       <c r="F24">
-        <v>0.70799999999999996</v>
+        <v>0.68899999999999995</v>
       </c>
       <c r="G24">
-        <v>0.72399999999999998</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="H24">
-        <v>0.53700000000000003</v>
+        <v>0.505</v>
       </c>
       <c r="I24">
-        <v>0.72399999999999998</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="J24">
-        <v>0.72399999999999998</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="K24">
-        <v>0.55800000000000005</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="L24">
-        <v>0.71099999999999997</v>
+        <v>0.69599999999999995</v>
       </c>
       <c r="M24">
-        <v>9.7999999999999997E-3</v>
+        <v>2.4E-2</v>
       </c>
       <c r="O24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -2089,37 +2166,37 @@
         <v>15</v>
       </c>
       <c r="D25">
-        <v>0.75700000000000001</v>
+        <v>0.751</v>
       </c>
       <c r="E25">
-        <v>0.70399999999999996</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="F25">
-        <v>0.75</v>
+        <v>0.74399999999999999</v>
       </c>
       <c r="G25">
-        <v>0.75700000000000001</v>
+        <v>0.751</v>
       </c>
       <c r="H25">
-        <v>0.64700000000000002</v>
+        <v>0.63</v>
       </c>
       <c r="I25">
-        <v>0.75700000000000001</v>
+        <v>0.751</v>
       </c>
       <c r="J25">
-        <v>0.75700000000000001</v>
+        <v>0.751</v>
       </c>
       <c r="K25">
-        <v>0.67100000000000004</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="L25">
-        <v>0.751</v>
+        <v>0.746</v>
       </c>
       <c r="M25">
-        <v>1.18E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2130,37 +2207,37 @@
         <v>14</v>
       </c>
       <c r="D26">
-        <v>0.71599999999999997</v>
+        <v>0.74</v>
       </c>
       <c r="E26">
-        <v>0.65100000000000002</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="F26">
-        <v>0.70899999999999996</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="G26">
-        <v>0.71599999999999997</v>
+        <v>0.74</v>
       </c>
       <c r="H26">
-        <v>0.54400000000000004</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="I26">
-        <v>0.71599999999999997</v>
+        <v>0.74</v>
       </c>
       <c r="J26">
-        <v>0.71599999999999997</v>
+        <v>0.74</v>
       </c>
       <c r="K26">
-        <v>0.57199999999999995</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="L26">
-        <v>0.70599999999999996</v>
+        <v>0.72699999999999998</v>
       </c>
       <c r="M26">
-        <v>1.7000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2171,37 +2248,37 @@
         <v>15</v>
       </c>
       <c r="D27">
+        <v>0.79</v>
+      </c>
+      <c r="E27">
+        <v>0.755</v>
+      </c>
+      <c r="F27">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="G27">
+        <v>0.79</v>
+      </c>
+      <c r="H27">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="I27">
+        <v>0.79</v>
+      </c>
+      <c r="J27">
+        <v>0.79</v>
+      </c>
+      <c r="K27">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="L27">
         <v>0.78500000000000003</v>
       </c>
-      <c r="E27">
-        <v>0.752</v>
-      </c>
-      <c r="F27">
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="G27">
-        <v>0.78500000000000003</v>
-      </c>
-      <c r="H27">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="I27">
-        <v>0.78500000000000003</v>
-      </c>
-      <c r="J27">
-        <v>0.78500000000000003</v>
-      </c>
-      <c r="K27">
-        <v>0.69899999999999995</v>
-      </c>
-      <c r="L27">
-        <v>0.78</v>
-      </c>
       <c r="M27">
-        <v>2.1999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2212,37 +2289,37 @@
         <v>14</v>
       </c>
       <c r="D28">
-        <v>0.73199999999999998</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="E28">
-        <v>0.73199999999999998</v>
+        <v>0.78</v>
       </c>
       <c r="F28">
-        <v>0.73799999999999999</v>
+        <v>0.745</v>
       </c>
       <c r="G28">
-        <v>0.73199999999999998</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="H28">
-        <v>0.52500000000000002</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="I28">
-        <v>0.73199999999999998</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="J28">
-        <v>0.73199999999999998</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="K28">
-        <v>0.54500000000000004</v>
+        <v>0.54300000000000004</v>
       </c>
       <c r="L28">
-        <v>0.71399999999999997</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="M28">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2253,37 +2330,37 @@
         <v>15</v>
       </c>
       <c r="D29">
-        <v>0.84499999999999997</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="E29">
-        <v>0.85399999999999998</v>
+        <v>0.85599999999999998</v>
       </c>
       <c r="F29">
-        <v>0.84799999999999998</v>
+        <v>0.84899999999999998</v>
       </c>
       <c r="G29">
-        <v>0.84499999999999997</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="H29">
-        <v>0.70699999999999996</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="I29">
-        <v>0.84499999999999997</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="J29">
-        <v>0.84499999999999997</v>
+        <v>0.84699999999999998</v>
       </c>
       <c r="K29">
         <v>0.747</v>
       </c>
       <c r="L29">
-        <v>0.83899999999999997</v>
+        <v>0.84</v>
       </c>
       <c r="M29">
-        <v>5.1999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -2294,34 +2371,34 @@
         <v>14</v>
       </c>
       <c r="D30">
-        <v>0.254</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="E30">
-        <v>0.17699999999999999</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="F30">
-        <v>0.25700000000000001</v>
+        <v>0.245</v>
       </c>
       <c r="G30">
-        <v>0.254</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="H30">
         <v>0.14099999999999999</v>
       </c>
       <c r="I30">
-        <v>0.254</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="J30">
-        <v>0.254</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="K30">
-        <v>0.14699999999999999</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="L30">
-        <v>0.24099999999999999</v>
+        <v>0.23699999999999999</v>
       </c>
       <c r="M30">
-        <v>5.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -2335,37 +2412,37 @@
         <v>15</v>
       </c>
       <c r="D31">
-        <v>0.40699999999999997</v>
+        <v>0.40799999999999997</v>
       </c>
       <c r="E31">
-        <v>0.4</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="F31">
-        <v>0.43099999999999999</v>
+        <v>0.434</v>
       </c>
       <c r="G31">
-        <v>0.40699999999999997</v>
+        <v>0.40799999999999997</v>
       </c>
       <c r="H31">
-        <v>0.26200000000000001</v>
+        <v>0.26</v>
       </c>
       <c r="I31">
-        <v>0.40699999999999997</v>
+        <v>0.40799999999999997</v>
       </c>
       <c r="J31">
-        <v>0.40699999999999997</v>
+        <v>0.40799999999999997</v>
       </c>
       <c r="K31">
-        <v>0.28899999999999998</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="L31">
         <v>0.39400000000000002</v>
       </c>
       <c r="M31">
-        <v>7.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -2376,34 +2453,34 @@
         <v>14</v>
       </c>
       <c r="D32">
-        <v>0.32800000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="E32">
-        <v>0.219</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="F32">
-        <v>0.314</v>
+        <v>0.3</v>
       </c>
       <c r="G32">
-        <v>0.32800000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="H32">
-        <v>0.19400000000000001</v>
+        <v>0.18</v>
       </c>
       <c r="I32">
-        <v>0.32800000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="J32">
-        <v>0.32800000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="K32">
-        <v>0.19900000000000001</v>
+        <v>0.182</v>
       </c>
       <c r="L32">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="M32">
-        <v>0.01</v>
+        <v>1.2E-2</v>
       </c>
       <c r="O32" t="s">
         <v>31</v>
@@ -2420,37 +2497,37 @@
         <v>15</v>
       </c>
       <c r="D33">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="E33">
         <v>0.52500000000000002</v>
       </c>
-      <c r="E33">
-        <v>0.51600000000000001</v>
-      </c>
       <c r="F33">
-        <v>0.54200000000000004</v>
+        <v>0.54900000000000004</v>
       </c>
       <c r="G33">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="H33">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="I33">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="J33">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="K33">
+        <v>0.43</v>
+      </c>
+      <c r="L33">
         <v>0.52500000000000002</v>
       </c>
-      <c r="H33">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="I33">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="J33">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="K33">
-        <v>0.41799999999999998</v>
-      </c>
-      <c r="L33">
-        <v>0.51700000000000002</v>
-      </c>
       <c r="M33">
-        <v>1.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -2461,34 +2538,34 @@
         <v>14</v>
       </c>
       <c r="D34">
-        <v>0.35399999999999998</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="E34">
-        <v>0.22500000000000001</v>
+        <v>0.217</v>
       </c>
       <c r="F34">
-        <v>0.34100000000000003</v>
+        <v>0.33900000000000002</v>
       </c>
       <c r="G34">
-        <v>0.35399999999999998</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="H34">
-        <v>0.21099999999999999</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="I34">
-        <v>0.35399999999999998</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="J34">
-        <v>0.35399999999999998</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="K34">
-        <v>0.21299999999999999</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="L34">
-        <v>0.34</v>
+        <v>0.33400000000000002</v>
       </c>
       <c r="M34">
-        <v>9.5999999999999992E-3</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2502,37 +2579,37 @@
         <v>15</v>
       </c>
       <c r="D35">
-        <v>0.622</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="E35">
-        <v>0.65500000000000003</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="F35">
-        <v>0.64600000000000002</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="G35">
-        <v>0.622</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="H35">
-        <v>0.45600000000000002</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="I35">
-        <v>0.622</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="J35">
-        <v>0.622</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="K35">
-        <v>0.497</v>
+        <v>0.495</v>
       </c>
       <c r="L35">
-        <v>0.61</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="M35">
-        <v>1.1599999999999999E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2543,31 +2620,31 @@
         <v>14</v>
       </c>
       <c r="D36">
-        <v>0.36199999999999999</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="E36">
-        <v>0.216</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="F36">
-        <v>0.35499999999999998</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="G36">
-        <v>0.36199999999999999</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="H36">
-        <v>0.19600000000000001</v>
+        <v>0.187</v>
       </c>
       <c r="I36">
-        <v>0.36199999999999999</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="J36">
-        <v>0.36199999999999999</v>
+        <v>0.35599999999999998</v>
       </c>
       <c r="K36">
-        <v>0.19600000000000001</v>
+        <v>0.186</v>
       </c>
       <c r="L36">
-        <v>0.34200000000000003</v>
+        <v>0.33100000000000002</v>
       </c>
       <c r="M36">
         <v>2.4E-2</v>
@@ -2584,37 +2661,37 @@
         <v>15</v>
       </c>
       <c r="D37">
-        <v>0.70699999999999996</v>
+        <v>0.71899999999999997</v>
       </c>
       <c r="E37">
-        <v>0.72399999999999998</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="F37">
-        <v>0.72799999999999998</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="G37">
-        <v>0.70699999999999996</v>
+        <v>0.71899999999999997</v>
       </c>
       <c r="H37">
-        <v>0.501</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="I37">
-        <v>0.70699999999999996</v>
+        <v>0.71899999999999997</v>
       </c>
       <c r="J37">
-        <v>0.70699999999999996</v>
+        <v>0.71899999999999997</v>
       </c>
       <c r="K37">
-        <v>0.54700000000000004</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="L37">
-        <v>0.69199999999999995</v>
+        <v>0.70299999999999996</v>
       </c>
       <c r="M37">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2625,34 +2702,34 @@
         <v>14</v>
       </c>
       <c r="D38">
-        <v>0.34799999999999998</v>
+        <v>0.34</v>
       </c>
       <c r="E38">
-        <v>0.20499999999999999</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="F38">
-        <v>0.34399999999999997</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="G38">
-        <v>0.34799999999999998</v>
+        <v>0.34</v>
       </c>
       <c r="H38">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="I38">
-        <v>0.34799999999999998</v>
+        <v>0.34</v>
       </c>
       <c r="J38">
-        <v>0.34799999999999998</v>
+        <v>0.34</v>
       </c>
       <c r="K38">
-        <v>0.18099999999999999</v>
+        <v>0.17</v>
       </c>
       <c r="L38">
-        <v>0.32400000000000001</v>
+        <v>0.312</v>
       </c>
       <c r="M38">
-        <v>2.7E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
@@ -2666,37 +2743,37 @@
         <v>15</v>
       </c>
       <c r="D39">
-        <v>0.71499999999999997</v>
+        <v>0.72299999999999998</v>
       </c>
       <c r="E39">
-        <v>0.73599999999999999</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="F39">
-        <v>0.74</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="G39">
-        <v>0.71499999999999997</v>
+        <v>0.72299999999999998</v>
       </c>
       <c r="H39">
-        <v>0.497</v>
+        <v>0.498</v>
       </c>
       <c r="I39">
-        <v>0.71499999999999997</v>
+        <v>0.72299999999999998</v>
       </c>
       <c r="J39">
-        <v>0.71499999999999997</v>
+        <v>0.72299999999999998</v>
       </c>
       <c r="K39">
-        <v>0.54200000000000004</v>
+        <v>0.54</v>
       </c>
       <c r="L39">
-        <v>0.69899999999999995</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="M39">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -2707,37 +2784,37 @@
         <v>14</v>
       </c>
       <c r="D40">
-        <v>0.72399999999999998</v>
+        <v>0.72</v>
       </c>
       <c r="E40">
-        <v>0.56000000000000005</v>
+        <v>0.58199999999999996</v>
       </c>
       <c r="F40">
-        <v>0.68899999999999995</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="G40">
-        <v>0.72399999999999998</v>
+        <v>0.72</v>
       </c>
       <c r="H40">
         <v>0.47499999999999998</v>
       </c>
       <c r="I40">
-        <v>0.72399999999999998</v>
+        <v>0.72</v>
       </c>
       <c r="J40">
-        <v>0.72399999999999998</v>
+        <v>0.72</v>
       </c>
       <c r="K40">
-        <v>0.49099999999999999</v>
+        <v>0.495</v>
       </c>
       <c r="L40">
-        <v>0.69099999999999995</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="M40">
-        <v>7.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -2748,37 +2825,37 @@
         <v>15</v>
       </c>
       <c r="D41">
-        <v>0.72299999999999998</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="E41">
-        <v>0.66300000000000003</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="F41">
-        <v>0.70699999999999996</v>
+        <v>0.71</v>
       </c>
       <c r="G41">
-        <v>0.72299999999999998</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="H41">
-        <v>0.54800000000000004</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="I41">
-        <v>0.72299999999999998</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="J41">
-        <v>0.72299999999999998</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="K41">
-        <v>0.58099999999999996</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="L41">
-        <v>0.70199999999999996</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="M41">
-        <v>7.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+        <v>5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -2819,7 +2896,7 @@
         <v>6.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -2860,7 +2937,7 @@
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -2871,37 +2948,37 @@
         <v>14</v>
       </c>
       <c r="D44">
-        <v>0.73399999999999999</v>
+        <v>0.746</v>
       </c>
       <c r="E44">
-        <v>0.68899999999999995</v>
+        <v>0.73</v>
       </c>
       <c r="F44">
-        <v>0.72699999999999998</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="G44">
-        <v>0.73399999999999999</v>
+        <v>0.746</v>
       </c>
       <c r="H44">
-        <v>0.58399999999999996</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="I44">
-        <v>0.73399999999999999</v>
+        <v>0.746</v>
       </c>
       <c r="J44">
-        <v>0.73399999999999999</v>
+        <v>0.746</v>
       </c>
       <c r="K44">
         <v>0.61799999999999999</v>
       </c>
       <c r="L44">
-        <v>0.72499999999999998</v>
+        <v>0.73399999999999999</v>
       </c>
       <c r="M44">
-        <v>1.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -2912,37 +2989,37 @@
         <v>15</v>
       </c>
       <c r="D45">
-        <v>0.79500000000000004</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="E45">
-        <v>0.76300000000000001</v>
+        <v>0.753</v>
       </c>
       <c r="F45">
-        <v>0.79100000000000004</v>
+        <v>0.78800000000000003</v>
       </c>
       <c r="G45">
-        <v>0.79500000000000004</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="H45">
-        <v>0.69499999999999995</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="I45">
-        <v>0.79500000000000004</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="J45">
-        <v>0.79500000000000004</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="K45">
-        <v>0.72299999999999998</v>
+        <v>0.71299999999999997</v>
       </c>
       <c r="L45">
-        <v>0.79100000000000004</v>
+        <v>0.78800000000000003</v>
       </c>
       <c r="M45">
-        <v>1.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -2953,37 +3030,37 @@
         <v>14</v>
       </c>
       <c r="D46">
-        <v>0.746</v>
+        <v>0.74</v>
       </c>
       <c r="E46">
-        <v>0.7</v>
+        <v>0.72699999999999998</v>
       </c>
       <c r="F46">
-        <v>0.74099999999999999</v>
+        <v>0.73799999999999999</v>
       </c>
       <c r="G46">
-        <v>0.746</v>
+        <v>0.74</v>
       </c>
       <c r="H46">
-        <v>0.56499999999999995</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="I46">
-        <v>0.746</v>
+        <v>0.74</v>
       </c>
       <c r="J46">
-        <v>0.746</v>
+        <v>0.74</v>
       </c>
       <c r="K46">
-        <v>0.59499999999999997</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="L46">
-        <v>0.73399999999999999</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="M46">
-        <v>1.7000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -2994,37 +3071,37 @@
         <v>15</v>
       </c>
       <c r="D47">
-        <v>0.85799999999999998</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="E47">
-        <v>0.85099999999999998</v>
+        <v>0.84299999999999997</v>
       </c>
       <c r="F47">
-        <v>0.85799999999999998</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="G47">
-        <v>0.85799999999999998</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="H47">
-        <v>0.78200000000000003</v>
+        <v>0.77900000000000003</v>
       </c>
       <c r="I47">
-        <v>0.85799999999999998</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="J47">
-        <v>0.85799999999999998</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="K47">
-        <v>0.81100000000000005</v>
+        <v>0.80600000000000005</v>
       </c>
       <c r="L47">
-        <v>0.85599999999999998</v>
+        <v>0.85699999999999998</v>
       </c>
       <c r="M47">
-        <v>1.9E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -3035,37 +3112,37 @@
         <v>14</v>
       </c>
       <c r="D48">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="E48">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="F48">
         <v>0.73399999999999999</v>
       </c>
-      <c r="E48">
-        <v>0.67700000000000005</v>
-      </c>
-      <c r="F48">
-        <v>0.73699999999999999</v>
-      </c>
       <c r="G48">
-        <v>0.73399999999999999</v>
+        <v>0.74199999999999999</v>
       </c>
       <c r="H48">
-        <v>0.57099999999999995</v>
+        <v>0.53600000000000003</v>
       </c>
       <c r="I48">
-        <v>0.73399999999999999</v>
+        <v>0.74199999999999999</v>
       </c>
       <c r="J48">
-        <v>0.73399999999999999</v>
+        <v>0.74199999999999999</v>
       </c>
       <c r="K48">
-        <v>0.59099999999999997</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="L48">
-        <v>0.72699999999999998</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="M48">
-        <v>2.2499999999999999E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -3076,34 +3153,34 @@
         <v>15</v>
       </c>
       <c r="D49">
-        <v>0.88300000000000001</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="E49">
-        <v>0.88300000000000001</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="F49">
         <v>0.88200000000000001</v>
       </c>
       <c r="G49">
-        <v>0.88300000000000001</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="H49">
-        <v>0.80100000000000005</v>
+        <v>0.80800000000000005</v>
       </c>
       <c r="I49">
-        <v>0.88300000000000001</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="J49">
-        <v>0.88300000000000001</v>
+        <v>0.88200000000000001</v>
       </c>
       <c r="K49">
-        <v>0.83399999999999996</v>
+        <v>0.83899999999999997</v>
       </c>
       <c r="L49">
-        <v>0.88100000000000001</v>
+        <v>0.88</v>
       </c>
       <c r="M49">
-        <v>2.9499999999999998E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -3191,20 +3268,7 @@
       <c r="C73" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M49" xr:uid="{3BBEE31F-A494-4277-82AD-63F056B36783}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="BNB_topics"/>
-        <filter val="DT_topics"/>
-        <filter val="MNB_topics"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="train"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M49" xr:uid="{3BBEE31F-A494-4277-82AD-63F056B36783}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3214,7 +3278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96611E49-C074-44E2-ADBF-AAB639D2C6AE}">
   <dimension ref="A2:V148"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A121" workbookViewId="0">
       <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Replaced table data again....
</commit_message>
<xml_diff>
--- a/data_dump.xlsx
+++ b/data_dump.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doodey\cs9414-opinion-mining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E97F80-C309-4EB0-918F-5D720692D0C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CD8406-D92B-4F63-A022-D710CB534E7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33915" yWindow="0" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
   </bookViews>
@@ -1073,10 +1073,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFAC374A-F1AE-473F-9409-AFFE657A853B}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AA73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1126,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1166,7 +1167,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1210,7 +1211,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1290,7 +1291,7 @@
         <v>4.3499999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1411,7 +1412,7 @@
         <v>0.11600000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1452,7 +1453,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1534,7 +1535,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1575,7 +1576,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1616,7 +1617,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1657,7 +1658,7 @@
         <v>8.9899999999999994E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>9.0899999999999995E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1739,7 +1740,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1780,7 +1781,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1821,7 +1822,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1865,7 +1866,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1906,7 +1907,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1947,7 +1948,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1988,7 +1989,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -2029,7 +2030,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -2070,7 +2071,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2155,7 +2156,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -2237,7 +2238,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2278,7 +2279,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2319,7 +2320,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2360,7 +2361,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -2401,7 +2402,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -2442,7 +2443,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -2486,7 +2487,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -2568,7 +2569,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2609,7 +2610,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2650,7 +2651,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2691,7 +2692,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2732,7 +2733,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -2773,7 +2774,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -2814,7 +2815,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -2855,7 +2856,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -2896,7 +2897,7 @@
         <v>6.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -2978,7 +2979,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -3019,7 +3020,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -3060,7 +3061,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -3101,7 +3102,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -3142,7 +3143,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -3268,7 +3269,18 @@
       <c r="C73" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M49" xr:uid="{3BBEE31F-A494-4277-82AD-63F056B36783}"/>
+  <autoFilter ref="A1:M49" xr:uid="{3BBEE31F-A494-4277-82AD-63F056B36783}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="400"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="test"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
GridsearchCV is legit but my PSO was better
</commit_message>
<xml_diff>
--- a/data_dump.xlsx
+++ b/data_dump.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doodey\cs9414-opinion-mining\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\King\cs9414-opinion-mining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262CE4B2-3E98-4BB7-8F79-F98C1737EA92}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130822CE-B6D4-426D-A9A8-396DF7F009EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{FA408021-59D1-4803-8533-1289EF066653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1073,10 +1073,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFAC374A-F1AE-473F-9409-AFFE657A853B}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AA73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,7 +1126,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1166,7 +1167,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1210,7 +1211,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1290,7 +1291,7 @@
         <v>4.3499999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1370,7 +1371,7 @@
         <v>4.4499999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1411,7 +1412,7 @@
         <v>0.11600000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1452,7 +1453,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1534,7 +1535,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1575,7 +1576,7 @@
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1616,7 +1617,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1657,7 +1658,7 @@
         <v>8.9899999999999994E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>9.0899999999999995E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1739,7 +1740,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1780,7 +1781,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1821,7 +1822,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1865,7 +1866,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1906,7 +1907,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1947,7 +1948,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1988,7 +1989,7 @@
         <v>5.5E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -2029,7 +2030,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -2070,7 +2071,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -2155,7 +2156,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -2196,7 +2197,7 @@
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -2237,7 +2238,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -2278,7 +2279,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2319,7 +2320,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -2360,7 +2361,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -2401,7 +2402,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -2442,7 +2443,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -2486,7 +2487,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -2527,7 +2528,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -2568,7 +2569,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -2609,7 +2610,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -2650,7 +2651,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -2691,7 +2692,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -2732,7 +2733,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -3268,6 +3269,13 @@
       <c r="C73" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M49" xr:uid="{32DB73BC-CB10-4260-A879-A3D3524548B6}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="MNB_sentiment"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>